<commit_message>
implement functions qlECBcode() and qlECBnextDate()
</commit_message>
<xml_diff>
--- a/Data2/XLS/EUR/EUR_JumpsQuotesFeedON.xlsx
+++ b/Data2/XLS/EUR/EUR_JumpsQuotesFeedON.xlsx
@@ -1674,11 +1674,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="38780288"/>
-        <c:axId val="38782080"/>
+        <c:axId val="133480448"/>
+        <c:axId val="133481984"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="38780288"/>
+        <c:axId val="133480448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1698,12 +1698,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="38782080"/>
+        <c:crossAx val="133481984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="38782080"/>
+        <c:axId val="133481984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1714,7 +1714,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="38780288"/>
+        <c:crossAx val="133480448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4871,11 +4871,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="38788480"/>
-        <c:axId val="84903040"/>
+        <c:axId val="211976192"/>
+        <c:axId val="211977728"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="38788480"/>
+        <c:axId val="211976192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4895,14 +4895,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84903040"/>
+        <c:crossAx val="211977728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="84903040"/>
+        <c:axId val="211977728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4913,7 +4913,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="38788480"/>
+        <c:crossAx val="211976192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5045,7 +5045,7 @@
       <sheetData sheetId="0">
         <row r="6">
           <cell r="D6">
-            <v>1</v>
+            <v>0</v>
           </cell>
         </row>
       </sheetData>
@@ -5669,7 +5669,7 @@
       </c>
       <c r="I8" s="60">
         <f>[1]!TriggerCounter</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8" s="58"/>
     </row>
@@ -5689,7 +5689,7 @@
       </c>
       <c r="I9" s="29">
         <f ca="1">_xll.ohTrigger(Contribution!M1)</f>
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="J9" s="4"/>
     </row>
@@ -5959,15 +5959,13 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D1"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" style="93" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="2" max="3" width="4" style="98" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="4" max="4" width="7" style="98" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="17.28515625" style="93" customWidth="1" outlineLevel="1"/>
+    <col min="2" max="3" width="4" style="98" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="4" width="7" style="98" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="21.42578125" style="93" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8" style="98" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.85546875" style="98" customWidth="1"/>
@@ -6038,9 +6036,9 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="125" t="e">
-        <f ca="1">_xll.qlECBNextDate(SettlementDate)</f>
-        <v>#NAME?</v>
+      <c r="A3" s="125">
+        <f>_xll.qlECBnextDate(Trigger,SettlementDate)</f>
+        <v>42256</v>
       </c>
       <c r="B3" s="161" t="s">
         <v>40</v>
@@ -6048,13 +6046,13 @@
       <c r="C3" s="161" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="80" t="e">
-        <f ca="1">_xll.qlECBcode(A3)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="E3" s="81" t="e">
-        <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
+      <c r="D3" s="80" t="str">
+        <f>_xll.qlECBcode(Trigger,A3)</f>
+        <v>SEP15</v>
+      </c>
+      <c r="E3" s="81" t="str">
+        <f t="shared" si="0"/>
+        <v>EURECBOISSEP15_Quote</v>
       </c>
       <c r="F3" s="81" t="e">
         <f ca="1">_xll.qlDatedOISRateHelper("W"&amp;Currency&amp;B3&amp;C3&amp;D3,A3,A4,E3,OvernightIndex)</f>
@@ -6081,9 +6079,9 @@
       <c r="L3" s="94"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="125" t="e">
-        <f ca="1">_xll.qlECBNextDate(A3)</f>
-        <v>#NAME?</v>
+      <c r="A4" s="125">
+        <f>_xll.qlECBnextDate(Trigger,A3)</f>
+        <v>42305</v>
       </c>
       <c r="B4" s="162" t="s">
         <v>40</v>
@@ -6091,13 +6089,13 @@
       <c r="C4" s="162" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="160" t="e">
-        <f ca="1">_xll.qlECBcode(A4)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="E4" s="85" t="e">
-        <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
+      <c r="D4" s="160" t="str">
+        <f>_xll.qlECBcode(Trigger,A4)</f>
+        <v>OCT15</v>
+      </c>
+      <c r="E4" s="85" t="str">
+        <f t="shared" si="0"/>
+        <v>EURECBOISOCT15_Quote</v>
       </c>
       <c r="F4" s="85" t="e">
         <f ca="1">_xll.qlDatedOISRateHelper("W"&amp;Currency&amp;B4&amp;C4&amp;D4,A4,A5,E4,OvernightIndex)</f>
@@ -6124,9 +6122,9 @@
       <c r="L4" s="95"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="125" t="e">
-        <f ca="1">_xll.qlECBNextDate(A4)</f>
-        <v>#NAME?</v>
+      <c r="A5" s="125">
+        <f>_xll.qlECBnextDate(Trigger,A4)</f>
+        <v>42347</v>
       </c>
       <c r="B5" s="162" t="s">
         <v>40</v>
@@ -6134,13 +6132,13 @@
       <c r="C5" s="162" t="s">
         <v>41</v>
       </c>
-      <c r="D5" s="160" t="e">
-        <f ca="1">_xll.qlECBcode(A5)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="E5" s="85" t="e">
-        <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
+      <c r="D5" s="160" t="str">
+        <f>_xll.qlECBcode(Trigger,A5)</f>
+        <v>DEC15</v>
+      </c>
+      <c r="E5" s="85" t="str">
+        <f t="shared" si="0"/>
+        <v>EURECBOISDEC15_Quote</v>
       </c>
       <c r="F5" s="85" t="e">
         <f ca="1">_xll.qlDatedOISRateHelper("W"&amp;Currency&amp;B5&amp;C5&amp;D5,A5,A6,E5,OvernightIndex)</f>
@@ -6166,9 +6164,9 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="125" t="e">
-        <f ca="1">_xll.qlECBNextDate(A5)</f>
-        <v>#NAME?</v>
+      <c r="A6" s="125">
+        <f>_xll.qlECBnextDate(Trigger,A5)</f>
+        <v>42395</v>
       </c>
       <c r="B6" s="162" t="s">
         <v>40</v>
@@ -6176,13 +6174,13 @@
       <c r="C6" s="162" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="160" t="e">
-        <f ca="1">_xll.qlECBcode(A6)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="E6" s="85" t="e">
-        <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
+      <c r="D6" s="160" t="str">
+        <f>_xll.qlECBcode(Trigger,A6)</f>
+        <v>JAN16</v>
+      </c>
+      <c r="E6" s="85" t="str">
+        <f t="shared" si="0"/>
+        <v>EURECBOISJAN16_Quote</v>
       </c>
       <c r="F6" s="85" t="e">
         <f ca="1">_xll.qlDatedOISRateHelper("W"&amp;Currency&amp;B6&amp;C6&amp;D6,A6,A7,E6,OvernightIndex)</f>
@@ -6208,9 +6206,9 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="125" t="e">
-        <f ca="1">_xll.qlECBNextDate(A6)</f>
-        <v>#NAME?</v>
+      <c r="A7" s="125">
+        <f>_xll.qlECBnextDate(Trigger,A6)</f>
+        <v>42445</v>
       </c>
       <c r="B7" s="162" t="s">
         <v>40</v>
@@ -6218,13 +6216,13 @@
       <c r="C7" s="162" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="160" t="e">
-        <f ca="1">_xll.qlECBcode(A7)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="E7" s="85" t="e">
-        <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
+      <c r="D7" s="160" t="str">
+        <f>_xll.qlECBcode(Trigger,A7)</f>
+        <v>MAR16</v>
+      </c>
+      <c r="E7" s="85" t="str">
+        <f t="shared" si="0"/>
+        <v>EURECBOISMAR16_Quote</v>
       </c>
       <c r="F7" s="85" t="e">
         <f ca="1">_xll.qlDatedOISRateHelper("W"&amp;Currency&amp;B7&amp;C7&amp;D7,A7,A8,E7,OvernightIndex)</f>
@@ -6250,9 +6248,9 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="125" t="e">
-        <f ca="1">_xll.qlECBNextDate(A7)</f>
-        <v>#NAME?</v>
+      <c r="A8" s="125">
+        <f>_xll.qlECBnextDate(Trigger,A7)</f>
+        <v>42487</v>
       </c>
       <c r="B8" s="162" t="s">
         <v>40</v>
@@ -6260,13 +6258,13 @@
       <c r="C8" s="162" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="160" t="e">
-        <f ca="1">_xll.qlECBcode(A8)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="E8" s="85" t="e">
-        <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
+      <c r="D8" s="160" t="str">
+        <f>_xll.qlECBcode(Trigger,A8)</f>
+        <v>APR16</v>
+      </c>
+      <c r="E8" s="85" t="str">
+        <f t="shared" si="0"/>
+        <v>EURECBOISAPR16_Quote</v>
       </c>
       <c r="F8" s="85" t="e">
         <f ca="1">_xll.qlDatedOISRateHelper("W"&amp;Currency&amp;B8&amp;C8&amp;D8,A8,A9,E8,OvernightIndex)</f>
@@ -6292,9 +6290,9 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="125" t="e">
-        <f ca="1">_xll.qlECBNextDate(A8)</f>
-        <v>#NAME?</v>
+      <c r="A9" s="125">
+        <f>_xll.qlECBnextDate(Trigger,A8)</f>
+        <v>42529</v>
       </c>
       <c r="B9" s="162" t="s">
         <v>40</v>
@@ -6302,13 +6300,13 @@
       <c r="C9" s="162" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="160" t="e">
-        <f ca="1">_xll.qlECBcode(A9)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="E9" s="85" t="e">
-        <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
+      <c r="D9" s="160" t="str">
+        <f>_xll.qlECBcode(Trigger,A9)</f>
+        <v>JUN16</v>
+      </c>
+      <c r="E9" s="85" t="str">
+        <f t="shared" si="0"/>
+        <v>EURECBOISJUN16_Quote</v>
       </c>
       <c r="F9" s="85" t="e">
         <f ca="1">_xll.qlDatedOISRateHelper("W"&amp;Currency&amp;B9&amp;C9&amp;D9,A9,A10,E9,OvernightIndex)</f>
@@ -6335,8 +6333,8 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="125" t="e">
-        <f ca="1">_xll.qlECBNextDate(A9)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlECBnextDate(Trigger,A9)</f>
+        <v>#NUM!</v>
       </c>
       <c r="B10" s="162" t="s">
         <v>40</v>
@@ -6345,12 +6343,12 @@
         <v>41</v>
       </c>
       <c r="D10" s="160" t="e">
-        <f ca="1">_xll.qlECBcode(A10)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlECBcode(Trigger,A10)</f>
+        <v>#NUM!</v>
       </c>
       <c r="E10" s="85" t="e">
-        <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
       </c>
       <c r="F10" s="85" t="e">
         <f ca="1">_xll.qlDatedOISRateHelper("W"&amp;Currency&amp;B10&amp;C10&amp;D10,A10,A11,E10,OvernightIndex)</f>
@@ -6377,8 +6375,8 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="125" t="e">
-        <f ca="1">_xll.qlECBNextDate(A10)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlECBnextDate(Trigger,A10)</f>
+        <v>#NUM!</v>
       </c>
       <c r="B11" s="162" t="s">
         <v>40</v>
@@ -6387,12 +6385,12 @@
         <v>41</v>
       </c>
       <c r="D11" s="160" t="e">
-        <f ca="1">_xll.qlECBcode(A11)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlECBcode(Trigger,A11)</f>
+        <v>#NUM!</v>
       </c>
       <c r="E11" s="85" t="e">
-        <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
       </c>
       <c r="F11" s="85" t="e">
         <f ca="1">_xll.qlDatedOISRateHelper("W"&amp;Currency&amp;B11&amp;C11&amp;D11,A11,A12,E11,OvernightIndex)</f>
@@ -6419,8 +6417,8 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="125" t="e">
-        <f ca="1">_xll.qlECBNextDate(A11)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlECBnextDate(Trigger,A11)</f>
+        <v>#NUM!</v>
       </c>
       <c r="B12" s="162" t="s">
         <v>40</v>
@@ -6429,12 +6427,12 @@
         <v>41</v>
       </c>
       <c r="D12" s="160" t="e">
-        <f ca="1">_xll.qlECBcode(A12)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlECBcode(Trigger,A12)</f>
+        <v>#NUM!</v>
       </c>
       <c r="E12" s="85" t="e">
-        <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
       </c>
       <c r="F12" s="85" t="e">
         <f ca="1">_xll.qlDatedOISRateHelper("W"&amp;Currency&amp;B12&amp;C12&amp;D12,A12,#REF!,E12,OvernightIndex)</f>
@@ -6467,13 +6465,13 @@
       <c r="C13" s="161" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="80" t="e">
-        <f t="array" ref="D13:D17">_xll.qlIMMNextCodes(_xll.qlSettingsEvaluationDate(Trigger)-1,$A13:$A17)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="E13" s="81" t="e">
+      <c r="D13" s="80" t="str">
+        <f t="array" ref="D13:D17">_xll.qlIMMNextCodes(Trigger,_xll.qlSettingsEvaluationDate(Trigger)-1,$A13:$A17)</f>
+        <v>U5</v>
+      </c>
+      <c r="E13" s="81" t="str">
         <f>Currency&amp;B13&amp;C13&amp;D13&amp;"_Quote"</f>
-        <v>#NUM!</v>
+        <v>EUROISU5_Quote</v>
       </c>
       <c r="F13" s="81" t="e">
         <f ca="1">_xll.qlFuturesRateHelper("W"&amp;Currency&amp;C13&amp;D13,E13,D13,PROPER(Currency)&amp;"ibor3M",0,,Trigger)</f>
@@ -6505,12 +6503,12 @@
       <c r="C14" s="162" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="160" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="E14" s="85" t="e">
+      <c r="D14" s="160" t="str">
+        <v>Z5</v>
+      </c>
+      <c r="E14" s="85" t="str">
         <f>Currency&amp;B14&amp;C14&amp;D14&amp;"_Quote"</f>
-        <v>#NUM!</v>
+        <v>EUROISZ5_Quote</v>
       </c>
       <c r="F14" s="85" t="e">
         <f ca="1">_xll.qlFuturesRateHelper("W"&amp;Currency&amp;C14&amp;D14,E14,D14,PROPER(Currency)&amp;"ibor3M",0,,Trigger)</f>
@@ -6542,12 +6540,12 @@
       <c r="C15" s="162" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="160" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="E15" s="85" t="e">
+      <c r="D15" s="160" t="str">
+        <v>H6</v>
+      </c>
+      <c r="E15" s="85" t="str">
         <f>Currency&amp;B15&amp;C15&amp;D15&amp;"_Quote"</f>
-        <v>#NUM!</v>
+        <v>EUROISH6_Quote</v>
       </c>
       <c r="F15" s="85" t="e">
         <f ca="1">_xll.qlFuturesRateHelper("W"&amp;Currency&amp;C15&amp;D15,E15,D15,PROPER(Currency)&amp;"ibor3M",0,,Trigger)</f>
@@ -6579,12 +6577,12 @@
       <c r="C16" s="162" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="160" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="E16" s="85" t="e">
+      <c r="D16" s="160" t="str">
+        <v>M6</v>
+      </c>
+      <c r="E16" s="85" t="str">
         <f>Currency&amp;B16&amp;C16&amp;D16&amp;"_Quote"</f>
-        <v>#NUM!</v>
+        <v>EUROISM6_Quote</v>
       </c>
       <c r="F16" s="85" t="e">
         <f ca="1">_xll.qlFuturesRateHelper("W"&amp;Currency&amp;C16&amp;D16,E16,D16,PROPER(Currency)&amp;"ibor3M",0,,Trigger)</f>
@@ -6616,12 +6614,12 @@
       <c r="C17" s="163" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="160" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="E17" s="85" t="e">
+      <c r="D17" s="160" t="str">
+        <v>U6</v>
+      </c>
+      <c r="E17" s="85" t="str">
         <f>Currency&amp;B17&amp;C17&amp;D17&amp;"_Quote"</f>
-        <v>#NUM!</v>
+        <v>EUROISU6_Quote</v>
       </c>
       <c r="F17" s="85" t="e">
         <f ca="1">_xll.qlFuturesRateHelper("W"&amp;Currency&amp;C17&amp;D17,E17,D17,PROPER(Currency)&amp;"ibor3M",0,,Trigger)</f>
@@ -7324,35 +7322,35 @@
     <row r="38" spans="2:11" x14ac:dyDescent="0.2">
       <c r="D38" s="93">
         <f ca="1">_xll.ohTrigger(RateHelpers)</f>
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E38" s="93">
         <f ca="1">_xll.ohTrigger(RateHelpers)</f>
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="F38" s="93">
         <f ca="1">_xll.ohTrigger(RateHelpers)</f>
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="G38" s="93">
         <f ca="1">_xll.ohTrigger(RateHelpers)</f>
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="H38" s="93">
         <f ca="1">_xll.ohTrigger(RateHelpers)</f>
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="I38" s="93">
         <f ca="1">_xll.ohTrigger(RateHelpers)</f>
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="J38" s="93">
         <f ca="1">_xll.ohTrigger(RateHelpers)</f>
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="K38" s="93">
         <f ca="1">_xll.ohTrigger(RateHelpers)</f>
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -33182,7 +33180,7 @@
       <c r="L1" s="22"/>
       <c r="M1" s="23">
         <f ca="1">_xll.ohTrigger(M3:M4)</f>
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="N1" s="144"/>
     </row>

</xml_diff>

<commit_message>
implement support for functions qlFuturesRateHelper(), qlOISRateHelper(), qlDatedOISRateHelper()
</commit_message>
<xml_diff>
--- a/Data2/XLS/EUR/EUR_JumpsQuotesFeedON.xlsx
+++ b/Data2/XLS/EUR/EUR_JumpsQuotesFeedON.xlsx
@@ -1674,11 +1674,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="133480448"/>
-        <c:axId val="133481984"/>
+        <c:axId val="214941696"/>
+        <c:axId val="214943232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="133480448"/>
+        <c:axId val="214941696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1698,12 +1698,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="133481984"/>
+        <c:crossAx val="214943232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="133481984"/>
+        <c:axId val="214943232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1714,7 +1714,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133480448"/>
+        <c:crossAx val="214941696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4871,11 +4871,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="211976192"/>
-        <c:axId val="211977728"/>
+        <c:axId val="221282304"/>
+        <c:axId val="221283840"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="211976192"/>
+        <c:axId val="221282304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4895,14 +4895,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="211977728"/>
+        <c:crossAx val="221283840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="211977728"/>
+        <c:axId val="221283840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4913,7 +4913,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="211976192"/>
+        <c:crossAx val="221282304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5045,7 +5045,7 @@
       <sheetData sheetId="0">
         <row r="6">
           <cell r="D6">
-            <v>0</v>
+            <v>4</v>
           </cell>
         </row>
       </sheetData>
@@ -5053,7 +5053,7 @@
       <sheetData sheetId="2">
         <row r="6">
           <cell r="D6" t="str">
-            <v>EUR6M#0001</v>
+            <v>EUR6M#0004</v>
           </cell>
         </row>
       </sheetData>
@@ -5088,7 +5088,7 @@
       <sheetData sheetId="7">
         <row r="6">
           <cell r="D6" t="str">
-            <v>EURTND_Quote#0001</v>
+            <v>EURTND_Quote#0004</v>
           </cell>
         </row>
       </sheetData>
@@ -5669,7 +5669,7 @@
       </c>
       <c r="I8" s="60">
         <f>[1]!TriggerCounter</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J8" s="58"/>
     </row>
@@ -5689,7 +5689,7 @@
       </c>
       <c r="I9" s="29">
         <f ca="1">_xll.ohTrigger(Contribution!M1)</f>
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="J9" s="4"/>
     </row>
@@ -5959,13 +5959,15 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" style="93" customWidth="1" outlineLevel="1"/>
-    <col min="2" max="3" width="4" style="98" customWidth="1" outlineLevel="1"/>
-    <col min="4" max="4" width="7" style="98" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" style="93" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="2" max="3" width="4" style="98" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="4" width="7" style="98" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="6" width="21.42578125" style="93" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8" style="98" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.85546875" style="98" customWidth="1"/>
@@ -6015,7 +6017,7 @@
       </c>
       <c r="F2" s="77" t="str">
         <f>_xll.qlFraRateHelper(EvaluationDate,"W"&amp;Currency&amp;B2&amp;C2&amp;D2,,,E2,"2d",OvernightIndex)</f>
-        <v>WEURSND#0000</v>
+        <v>WEURSND#0008</v>
       </c>
       <c r="G2" s="78" t="b">
         <v>0</v>
@@ -6054,13 +6056,13 @@
         <f t="shared" si="0"/>
         <v>EURECBOISSEP15_Quote</v>
       </c>
-      <c r="F3" s="81" t="e">
-        <f ca="1">_xll.qlDatedOISRateHelper("W"&amp;Currency&amp;B3&amp;C3&amp;D3,A3,A4,E3,OvernightIndex)</f>
-        <v>#NAME?</v>
+      <c r="F3" s="81" t="str">
+        <f>_xll.qlDatedOISRateHelper(Trigger,"W"&amp;Currency&amp;B3&amp;C3&amp;D3,,,A3,A4,E3,OvernightIndex)</f>
+        <v>WEURECBOISSEP15#0003</v>
       </c>
       <c r="G3" s="82" t="b">
-        <f ca="1">IF(ISERROR(F3),FALSE,TRUE)</f>
-        <v>0</v>
+        <f>IF(ISERROR(F3),FALSE,TRUE)</f>
+        <v>1</v>
       </c>
       <c r="H3" s="83">
         <v>70</v>
@@ -6097,13 +6099,13 @@
         <f t="shared" si="0"/>
         <v>EURECBOISOCT15_Quote</v>
       </c>
-      <c r="F4" s="85" t="e">
-        <f ca="1">_xll.qlDatedOISRateHelper("W"&amp;Currency&amp;B4&amp;C4&amp;D4,A4,A5,E4,OvernightIndex)</f>
-        <v>#NAME?</v>
+      <c r="F4" s="85" t="str">
+        <f>_xll.qlDatedOISRateHelper(Trigger,"W"&amp;Currency&amp;B4&amp;C4&amp;D4,,,A4,A5,E4,OvernightIndex)</f>
+        <v>WEURECBOISOCT15#0003</v>
       </c>
       <c r="G4" s="82" t="b">
-        <f t="shared" ref="G4:G12" ca="1" si="1">IF(ISERROR(F4),FALSE,TRUE)</f>
-        <v>0</v>
+        <f t="shared" ref="G4:G12" si="1">IF(ISERROR(F4),FALSE,TRUE)</f>
+        <v>1</v>
       </c>
       <c r="H4" s="82">
         <v>70</v>
@@ -6140,13 +6142,13 @@
         <f t="shared" si="0"/>
         <v>EURECBOISDEC15_Quote</v>
       </c>
-      <c r="F5" s="85" t="e">
-        <f ca="1">_xll.qlDatedOISRateHelper("W"&amp;Currency&amp;B5&amp;C5&amp;D5,A5,A6,E5,OvernightIndex)</f>
-        <v>#NAME?</v>
+      <c r="F5" s="85" t="str">
+        <f>_xll.qlDatedOISRateHelper(Trigger,"W"&amp;Currency&amp;B5&amp;C5&amp;D5,,,A5,A6,E5,OvernightIndex)</f>
+        <v>WEURECBOISDEC15#0003</v>
       </c>
       <c r="G5" s="82" t="b">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="H5" s="82">
         <v>70</v>
@@ -6182,13 +6184,13 @@
         <f t="shared" si="0"/>
         <v>EURECBOISJAN16_Quote</v>
       </c>
-      <c r="F6" s="85" t="e">
-        <f ca="1">_xll.qlDatedOISRateHelper("W"&amp;Currency&amp;B6&amp;C6&amp;D6,A6,A7,E6,OvernightIndex)</f>
-        <v>#NAME?</v>
+      <c r="F6" s="85" t="str">
+        <f>_xll.qlDatedOISRateHelper(Trigger,"W"&amp;Currency&amp;B6&amp;C6&amp;D6,,,A6,A7,E6,OvernightIndex)</f>
+        <v>WEURECBOISJAN16#0003</v>
       </c>
       <c r="G6" s="82" t="b">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="H6" s="82">
         <v>70</v>
@@ -6224,13 +6226,13 @@
         <f t="shared" si="0"/>
         <v>EURECBOISMAR16_Quote</v>
       </c>
-      <c r="F7" s="85" t="e">
-        <f ca="1">_xll.qlDatedOISRateHelper("W"&amp;Currency&amp;B7&amp;C7&amp;D7,A7,A8,E7,OvernightIndex)</f>
-        <v>#NAME?</v>
+      <c r="F7" s="85" t="str">
+        <f>_xll.qlDatedOISRateHelper(Trigger,"W"&amp;Currency&amp;B7&amp;C7&amp;D7,,,A7,A8,E7,OvernightIndex)</f>
+        <v>WEURECBOISMAR16#0003</v>
       </c>
       <c r="G7" s="82" t="b">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="H7" s="82">
         <v>70</v>
@@ -6266,13 +6268,13 @@
         <f t="shared" si="0"/>
         <v>EURECBOISAPR16_Quote</v>
       </c>
-      <c r="F8" s="85" t="e">
-        <f ca="1">_xll.qlDatedOISRateHelper("W"&amp;Currency&amp;B8&amp;C8&amp;D8,A8,A9,E8,OvernightIndex)</f>
-        <v>#NAME?</v>
+      <c r="F8" s="85" t="str">
+        <f>_xll.qlDatedOISRateHelper(Trigger,"W"&amp;Currency&amp;B8&amp;C8&amp;D8,,,A8,A9,E8,OvernightIndex)</f>
+        <v>WEURECBOISAPR16#0003</v>
       </c>
       <c r="G8" s="82" t="b">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="H8" s="82">
         <v>70</v>
@@ -6309,11 +6311,11 @@
         <v>EURECBOISJUN16_Quote</v>
       </c>
       <c r="F9" s="85" t="e">
-        <f ca="1">_xll.qlDatedOISRateHelper("W"&amp;Currency&amp;B9&amp;C9&amp;D9,A9,A10,E9,OvernightIndex)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlDatedOISRateHelper(Trigger,"W"&amp;Currency&amp;B9&amp;C9&amp;D9,,,A9,A10,E9,OvernightIndex)</f>
+        <v>#NUM!</v>
       </c>
       <c r="G9" s="82" t="b">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H9" s="82">
@@ -6351,11 +6353,11 @@
         <v>#NUM!</v>
       </c>
       <c r="F10" s="85" t="e">
-        <f ca="1">_xll.qlDatedOISRateHelper("W"&amp;Currency&amp;B10&amp;C10&amp;D10,A10,A11,E10,OvernightIndex)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlDatedOISRateHelper(Trigger,"W"&amp;Currency&amp;B10&amp;C10&amp;D10,,,A10,A11,E10,OvernightIndex)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="G10" s="82" t="b">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H10" s="82">
@@ -6393,11 +6395,11 @@
         <v>#NUM!</v>
       </c>
       <c r="F11" s="85" t="e">
-        <f ca="1">_xll.qlDatedOISRateHelper("W"&amp;Currency&amp;B11&amp;C11&amp;D11,A11,A12,E11,OvernightIndex)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlDatedOISRateHelper(Trigger,"W"&amp;Currency&amp;B11&amp;C11&amp;D11,,,A11,A12,E11,OvernightIndex)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="G11" s="82" t="b">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H11" s="82">
@@ -6435,11 +6437,11 @@
         <v>#NUM!</v>
       </c>
       <c r="F12" s="85" t="e">
-        <f ca="1">_xll.qlDatedOISRateHelper("W"&amp;Currency&amp;B12&amp;C12&amp;D12,A12,#REF!,E12,OvernightIndex)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlDatedOISRateHelper(Trigger,"W"&amp;Currency&amp;B12&amp;C12&amp;D12,,,A12,A13,E12,OvernightIndex)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="G12" s="82" t="b">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H12" s="82">
@@ -6474,8 +6476,8 @@
         <v>EUROISU5_Quote</v>
       </c>
       <c r="F13" s="81" t="e">
-        <f ca="1">_xll.qlFuturesRateHelper("W"&amp;Currency&amp;C13&amp;D13,E13,D13,PROPER(Currency)&amp;"ibor3M",0,,Trigger)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlFuturesRateHelper(Trigger,"W"&amp;Currency&amp;C13&amp;D13,,,E13,"IMM",D13,PROPER(Currency)&amp;"ibor3M",0)</f>
+        <v>#NUM!</v>
       </c>
       <c r="G13" s="83" t="b">
         <v>0</v>
@@ -6511,8 +6513,8 @@
         <v>EUROISZ5_Quote</v>
       </c>
       <c r="F14" s="85" t="e">
-        <f ca="1">_xll.qlFuturesRateHelper("W"&amp;Currency&amp;C14&amp;D14,E14,D14,PROPER(Currency)&amp;"ibor3M",0,,Trigger)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlFuturesRateHelper(Trigger,"W"&amp;Currency&amp;C14&amp;D14,,,E14,"IMM",D14,PROPER(Currency)&amp;"ibor3M",0)</f>
+        <v>#NUM!</v>
       </c>
       <c r="G14" s="82" t="b">
         <v>0</v>
@@ -6548,8 +6550,8 @@
         <v>EUROISH6_Quote</v>
       </c>
       <c r="F15" s="85" t="e">
-        <f ca="1">_xll.qlFuturesRateHelper("W"&amp;Currency&amp;C15&amp;D15,E15,D15,PROPER(Currency)&amp;"ibor3M",0,,Trigger)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlFuturesRateHelper(Trigger,"W"&amp;Currency&amp;C15&amp;D15,,,E15,"IMM",D15,PROPER(Currency)&amp;"ibor3M",0)</f>
+        <v>#NUM!</v>
       </c>
       <c r="G15" s="82" t="b">
         <v>0</v>
@@ -6585,8 +6587,8 @@
         <v>EUROISM6_Quote</v>
       </c>
       <c r="F16" s="85" t="e">
-        <f ca="1">_xll.qlFuturesRateHelper("W"&amp;Currency&amp;C16&amp;D16,E16,D16,PROPER(Currency)&amp;"ibor3M",0,,Trigger)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlFuturesRateHelper(Trigger,"W"&amp;Currency&amp;C16&amp;D16,,,E16,"IMM",D16,PROPER(Currency)&amp;"ibor3M",0)</f>
+        <v>#NUM!</v>
       </c>
       <c r="G16" s="82" t="b">
         <v>0</v>
@@ -6622,8 +6624,8 @@
         <v>EUROISU6_Quote</v>
       </c>
       <c r="F17" s="85" t="e">
-        <f ca="1">_xll.qlFuturesRateHelper("W"&amp;Currency&amp;C17&amp;D17,E17,D17,PROPER(Currency)&amp;"ibor3M",0,,Trigger)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlFuturesRateHelper(Trigger,"W"&amp;Currency&amp;C17&amp;D17,,,E17,"IMM",D17,PROPER(Currency)&amp;"ibor3M",0)</f>
+        <v>#NUM!</v>
       </c>
       <c r="G17" s="82" t="b">
         <v>0</v>
@@ -6657,9 +6659,9 @@
         <f t="shared" si="0"/>
         <v>EUREONSW_Quote</v>
       </c>
-      <c r="F18" s="81" t="e">
-        <f ca="1">_xll.qlOISRateHelper("W"&amp;Currency&amp;B18&amp;C18&amp;D18,2,"1w",E18,OvernightIndex,,EvaluationDate)</f>
-        <v>#NAME?</v>
+      <c r="F18" s="81" t="str">
+        <f>_xll.qlOISRateHelper(EvaluationDate,"W"&amp;Currency&amp;B18&amp;C18&amp;D18,,,2,"1w",E18,OvernightIndex)</f>
+        <v>WEUREONSW#0001</v>
       </c>
       <c r="G18" s="83" t="b">
         <v>1</v>
@@ -6692,9 +6694,9 @@
         <f t="shared" si="0"/>
         <v>EUREON2W_Quote</v>
       </c>
-      <c r="F19" s="85" t="e">
-        <f ca="1">_xll.qlOISRateHelper("W"&amp;Currency&amp;B19&amp;C19&amp;D19,2,D19,E19,OvernightIndex,,EvaluationDate)</f>
-        <v>#NAME?</v>
+      <c r="F19" s="85" t="str">
+        <f>_xll.qlOISRateHelper(EvaluationDate,"W"&amp;Currency&amp;B19&amp;C19&amp;D19,,,2,"1w",E19,OvernightIndex)</f>
+        <v>WEUREON2W#0001</v>
       </c>
       <c r="G19" s="82" t="b">
         <v>1</v>
@@ -6727,9 +6729,9 @@
         <f t="shared" si="0"/>
         <v>EUREON3W_Quote</v>
       </c>
-      <c r="F20" s="85" t="e">
-        <f ca="1">_xll.qlOISRateHelper("W"&amp;Currency&amp;B20&amp;C20&amp;D20,2,D20,E20,OvernightIndex,,EvaluationDate)</f>
-        <v>#NAME?</v>
+      <c r="F20" s="85" t="str">
+        <f>_xll.qlOISRateHelper(EvaluationDate,"W"&amp;Currency&amp;B20&amp;C20&amp;D20,,,2,"1w",E20,OvernightIndex)</f>
+        <v>WEUREON3W#0001</v>
       </c>
       <c r="G20" s="82" t="b">
         <v>1</v>
@@ -6762,9 +6764,9 @@
         <f t="shared" si="0"/>
         <v>EUREON1M_Quote</v>
       </c>
-      <c r="F21" s="85" t="e">
-        <f ca="1">_xll.qlOISRateHelper("W"&amp;Currency&amp;B21&amp;C21&amp;D21,2,D21,E21,OvernightIndex,,EvaluationDate)</f>
-        <v>#NAME?</v>
+      <c r="F21" s="85" t="str">
+        <f>_xll.qlOISRateHelper(EvaluationDate,"W"&amp;Currency&amp;B21&amp;C21&amp;D21,,,2,"1w",E21,OvernightIndex)</f>
+        <v>WEUREON1M#0001</v>
       </c>
       <c r="G21" s="82" t="b">
         <v>1</v>
@@ -6797,9 +6799,9 @@
         <f t="shared" si="0"/>
         <v>EUREON2M_Quote</v>
       </c>
-      <c r="F22" s="85" t="e">
-        <f ca="1">_xll.qlOISRateHelper("W"&amp;Currency&amp;B22&amp;C22&amp;D22,2,D22,E22,OvernightIndex,,EvaluationDate)</f>
-        <v>#NAME?</v>
+      <c r="F22" s="85" t="str">
+        <f>_xll.qlOISRateHelper(EvaluationDate,"W"&amp;Currency&amp;B22&amp;C22&amp;D22,,,2,"1w",E22,OvernightIndex)</f>
+        <v>WEUREON2M#0001</v>
       </c>
       <c r="G22" s="82" t="b">
         <v>1</v>
@@ -6832,9 +6834,9 @@
         <f t="shared" si="0"/>
         <v>EUREON3M_Quote</v>
       </c>
-      <c r="F23" s="85" t="e">
-        <f ca="1">_xll.qlOISRateHelper("W"&amp;Currency&amp;B23&amp;C23&amp;D23,2,D23,E23,OvernightIndex,,EvaluationDate)</f>
-        <v>#NAME?</v>
+      <c r="F23" s="85" t="str">
+        <f>_xll.qlOISRateHelper(EvaluationDate,"W"&amp;Currency&amp;B23&amp;C23&amp;D23,,,2,"1w",E23,OvernightIndex)</f>
+        <v>WEUREON3M#0001</v>
       </c>
       <c r="G23" s="82" t="b">
         <v>1</v>
@@ -6867,9 +6869,9 @@
         <f t="shared" si="0"/>
         <v>EUREON4M_Quote</v>
       </c>
-      <c r="F24" s="85" t="e">
-        <f ca="1">_xll.qlOISRateHelper("W"&amp;Currency&amp;B24&amp;C24&amp;D24,2,D24,E24,OvernightIndex,,EvaluationDate)</f>
-        <v>#NAME?</v>
+      <c r="F24" s="85" t="str">
+        <f>_xll.qlOISRateHelper(EvaluationDate,"W"&amp;Currency&amp;B24&amp;C24&amp;D24,,,2,"1w",E24,OvernightIndex)</f>
+        <v>WEUREON4M#0001</v>
       </c>
       <c r="G24" s="82" t="b">
         <v>1</v>
@@ -6902,9 +6904,9 @@
         <f t="shared" si="0"/>
         <v>EUREON5M_Quote</v>
       </c>
-      <c r="F25" s="85" t="e">
-        <f ca="1">_xll.qlOISRateHelper("W"&amp;Currency&amp;B25&amp;C25&amp;D25,2,D25,E25,OvernightIndex,,EvaluationDate)</f>
-        <v>#NAME?</v>
+      <c r="F25" s="85" t="str">
+        <f>_xll.qlOISRateHelper(EvaluationDate,"W"&amp;Currency&amp;B25&amp;C25&amp;D25,,,2,"1w",E25,OvernightIndex)</f>
+        <v>WEUREON5M#0001</v>
       </c>
       <c r="G25" s="82" t="b">
         <v>1</v>
@@ -6937,9 +6939,9 @@
         <f t="shared" si="0"/>
         <v>EUREON6M_Quote</v>
       </c>
-      <c r="F26" s="85" t="e">
-        <f ca="1">_xll.qlOISRateHelper("W"&amp;Currency&amp;B26&amp;C26&amp;D26,2,D26,E26,OvernightIndex,,EvaluationDate)</f>
-        <v>#NAME?</v>
+      <c r="F26" s="85" t="str">
+        <f>_xll.qlOISRateHelper(EvaluationDate,"W"&amp;Currency&amp;B26&amp;C26&amp;D26,,,2,"1w",E26,OvernightIndex)</f>
+        <v>WEUREON6M#0001</v>
       </c>
       <c r="G26" s="82" t="b">
         <v>1</v>
@@ -6972,9 +6974,9 @@
         <f t="shared" si="0"/>
         <v>EUREON7M_Quote</v>
       </c>
-      <c r="F27" s="85" t="e">
-        <f ca="1">_xll.qlOISRateHelper("W"&amp;Currency&amp;B27&amp;C27&amp;D27,2,D27,E27,OvernightIndex,,EvaluationDate)</f>
-        <v>#NAME?</v>
+      <c r="F27" s="85" t="str">
+        <f>_xll.qlOISRateHelper(EvaluationDate,"W"&amp;Currency&amp;B27&amp;C27&amp;D27,,,2,"1w",E27,OvernightIndex)</f>
+        <v>WEUREON7M#0001</v>
       </c>
       <c r="G27" s="82" t="b">
         <v>1</v>
@@ -7007,9 +7009,9 @@
         <f t="shared" si="0"/>
         <v>EUREON8M_Quote</v>
       </c>
-      <c r="F28" s="85" t="e">
-        <f ca="1">_xll.qlOISRateHelper("W"&amp;Currency&amp;B28&amp;C28&amp;D28,2,D28,E28,OvernightIndex,,EvaluationDate)</f>
-        <v>#NAME?</v>
+      <c r="F28" s="85" t="str">
+        <f>_xll.qlOISRateHelper(EvaluationDate,"W"&amp;Currency&amp;B28&amp;C28&amp;D28,,,2,"1w",E28,OvernightIndex)</f>
+        <v>WEUREON8M#0001</v>
       </c>
       <c r="G28" s="82" t="b">
         <v>1</v>
@@ -7042,9 +7044,9 @@
         <f t="shared" si="0"/>
         <v>EUREON9M_Quote</v>
       </c>
-      <c r="F29" s="85" t="e">
-        <f ca="1">_xll.qlOISRateHelper("W"&amp;Currency&amp;B29&amp;C29&amp;D29,2,D29,E29,OvernightIndex,,EvaluationDate)</f>
-        <v>#NAME?</v>
+      <c r="F29" s="85" t="str">
+        <f>_xll.qlOISRateHelper(EvaluationDate,"W"&amp;Currency&amp;B29&amp;C29&amp;D29,,,2,"1w",E29,OvernightIndex)</f>
+        <v>WEUREON9M#0001</v>
       </c>
       <c r="G29" s="82" t="b">
         <v>1</v>
@@ -7077,9 +7079,9 @@
         <f t="shared" si="0"/>
         <v>EUREON10M_Quote</v>
       </c>
-      <c r="F30" s="85" t="e">
-        <f ca="1">_xll.qlOISRateHelper("W"&amp;Currency&amp;B30&amp;C30&amp;D30,2,D30,E30,OvernightIndex,,EvaluationDate)</f>
-        <v>#NAME?</v>
+      <c r="F30" s="85" t="str">
+        <f>_xll.qlOISRateHelper(EvaluationDate,"W"&amp;Currency&amp;B30&amp;C30&amp;D30,,,2,"1w",E30,OvernightIndex)</f>
+        <v>WEUREON10M#0001</v>
       </c>
       <c r="G30" s="82" t="b">
         <v>1</v>
@@ -7112,9 +7114,9 @@
         <f t="shared" si="0"/>
         <v>EUREON11M_Quote</v>
       </c>
-      <c r="F31" s="85" t="e">
-        <f ca="1">_xll.qlOISRateHelper("W"&amp;Currency&amp;B31&amp;C31&amp;D31,2,D31,E31,OvernightIndex,,EvaluationDate)</f>
-        <v>#NAME?</v>
+      <c r="F31" s="85" t="str">
+        <f>_xll.qlOISRateHelper(EvaluationDate,"W"&amp;Currency&amp;B31&amp;C31&amp;D31,,,2,"1w",E31,OvernightIndex)</f>
+        <v>WEUREON11M#0001</v>
       </c>
       <c r="G31" s="82" t="b">
         <v>1</v>
@@ -7147,9 +7149,9 @@
         <f t="shared" si="0"/>
         <v>EUREON1Y_Quote</v>
       </c>
-      <c r="F32" s="85" t="e">
-        <f ca="1">_xll.qlOISRateHelper("W"&amp;Currency&amp;B32&amp;C32&amp;D32,2,D32,E32,OvernightIndex,,EvaluationDate)</f>
-        <v>#NAME?</v>
+      <c r="F32" s="85" t="str">
+        <f>_xll.qlOISRateHelper(EvaluationDate,"W"&amp;Currency&amp;B32&amp;C32&amp;D32,,,2,"1w",E32,OvernightIndex)</f>
+        <v>WEUREON1Y#0001</v>
       </c>
       <c r="G32" s="82" t="b">
         <v>1</v>
@@ -7182,9 +7184,9 @@
         <f t="shared" si="0"/>
         <v>EUREON15M_Quote</v>
       </c>
-      <c r="F33" s="85" t="e">
-        <f ca="1">_xll.qlOISRateHelper("W"&amp;Currency&amp;B33&amp;C33&amp;D33,2,D33,E33,OvernightIndex,,EvaluationDate)</f>
-        <v>#NAME?</v>
+      <c r="F33" s="85" t="str">
+        <f>_xll.qlOISRateHelper(EvaluationDate,"W"&amp;Currency&amp;B33&amp;C33&amp;D33,,,2,"1w",E33,OvernightIndex)</f>
+        <v>WEUREON15M#0001</v>
       </c>
       <c r="G33" s="82" t="b">
         <v>1</v>
@@ -7217,9 +7219,9 @@
         <f t="shared" si="0"/>
         <v>EUREON18M_Quote</v>
       </c>
-      <c r="F34" s="85" t="e">
-        <f ca="1">_xll.qlOISRateHelper("W"&amp;Currency&amp;B34&amp;C34&amp;D34,2,D34,E34,OvernightIndex,,EvaluationDate)</f>
-        <v>#NAME?</v>
+      <c r="F34" s="85" t="str">
+        <f>_xll.qlOISRateHelper(EvaluationDate,"W"&amp;Currency&amp;B34&amp;C34&amp;D34,,,2,"1w",E34,OvernightIndex)</f>
+        <v>WEUREON18M#0001</v>
       </c>
       <c r="G34" s="82" t="b">
         <v>1</v>
@@ -7252,9 +7254,9 @@
         <f t="shared" si="0"/>
         <v>EUREON21M_Quote</v>
       </c>
-      <c r="F35" s="85" t="e">
-        <f ca="1">_xll.qlOISRateHelper("W"&amp;Currency&amp;B35&amp;C35&amp;D35,2,D35,E35,OvernightIndex,,EvaluationDate)</f>
-        <v>#NAME?</v>
+      <c r="F35" s="85" t="str">
+        <f>_xll.qlOISRateHelper(EvaluationDate,"W"&amp;Currency&amp;B35&amp;C35&amp;D35,,,2,"1w",E35,OvernightIndex)</f>
+        <v>WEUREON21M#0001</v>
       </c>
       <c r="G35" s="82" t="b">
         <v>1</v>
@@ -7287,9 +7289,9 @@
         <f t="shared" si="0"/>
         <v>EUREON2Y_Quote</v>
       </c>
-      <c r="F36" s="90" t="e">
-        <f ca="1">_xll.qlOISRateHelper("W"&amp;Currency&amp;B36&amp;C36&amp;D36,2,D36,E36,OvernightIndex,,EvaluationDate)</f>
-        <v>#NAME?</v>
+      <c r="F36" s="90" t="str">
+        <f>_xll.qlOISRateHelper(EvaluationDate,"W"&amp;Currency&amp;B36&amp;C36&amp;D36,,,2,"1w",E36,OvernightIndex)</f>
+        <v>WEUREON2Y#0001</v>
       </c>
       <c r="G36" s="91" t="b">
         <v>1</v>
@@ -7321,36 +7323,36 @@
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.2">
       <c r="D38" s="93">
-        <f ca="1">_xll.ohTrigger(RateHelpers)</f>
-        <v>12</v>
+        <f>_xll.ohTrigger(RateHelpers)</f>
+        <v>13</v>
       </c>
       <c r="E38" s="93">
-        <f ca="1">_xll.ohTrigger(RateHelpers)</f>
-        <v>12</v>
+        <f>_xll.ohTrigger(RateHelpers)</f>
+        <v>13</v>
       </c>
       <c r="F38" s="93">
-        <f ca="1">_xll.ohTrigger(RateHelpers)</f>
-        <v>12</v>
+        <f>_xll.ohTrigger(RateHelpers)</f>
+        <v>13</v>
       </c>
       <c r="G38" s="93">
-        <f ca="1">_xll.ohTrigger(RateHelpers)</f>
-        <v>12</v>
+        <f>_xll.ohTrigger(RateHelpers)</f>
+        <v>13</v>
       </c>
       <c r="H38" s="93">
-        <f ca="1">_xll.ohTrigger(RateHelpers)</f>
-        <v>12</v>
+        <f>_xll.ohTrigger(RateHelpers)</f>
+        <v>13</v>
       </c>
       <c r="I38" s="93">
-        <f ca="1">_xll.ohTrigger(RateHelpers)</f>
-        <v>12</v>
+        <f>_xll.ohTrigger(RateHelpers)</f>
+        <v>13</v>
       </c>
       <c r="J38" s="93">
-        <f ca="1">_xll.ohTrigger(RateHelpers)</f>
-        <v>12</v>
+        <f>_xll.ohTrigger(RateHelpers)</f>
+        <v>13</v>
       </c>
       <c r="K38" s="93">
-        <f ca="1">_xll.ohTrigger(RateHelpers)</f>
-        <v>12</v>
+        <f>_xll.ohTrigger(RateHelpers)</f>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -33180,7 +33182,7 @@
       <c r="L1" s="22"/>
       <c r="M1" s="23">
         <f ca="1">_xll.ohTrigger(M3:M4)</f>
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="N1" s="144"/>
     </row>
@@ -33254,7 +33256,7 @@
       </c>
       <c r="K3" s="40" t="str">
         <f>_xll.qlSimpleQuote(Trigger,J3,,TRUE)</f>
-        <v>EURJump1_SYNTHON_Quote#0001</v>
+        <v>EURJump1_SYNTHON_Quote#0004</v>
       </c>
       <c r="L3" s="40" t="e">
         <f t="array" aca="1" ref="L3:L15" ca="1">QuoteLive</f>
@@ -33306,7 +33308,7 @@
       </c>
       <c r="K4" s="141" t="str">
         <f>_xll.qlSimpleQuote(Trigger,J4,,TRUE)</f>
-        <v>EURJump2_SYNTHON_Quote#0001</v>
+        <v>EURJump2_SYNTHON_Quote#0004</v>
       </c>
       <c r="L4" s="141" t="e">
         <f ca="1"/>
@@ -33358,7 +33360,7 @@
       </c>
       <c r="K5" s="141" t="str">
         <f>_xll.qlSimpleQuote(Trigger,J5,,TRUE)</f>
-        <v>EURJump3_SYNTHON_Quote#0001</v>
+        <v>EURJump3_SYNTHON_Quote#0004</v>
       </c>
       <c r="L5" s="141" t="e">
         <f ca="1"/>
@@ -33410,7 +33412,7 @@
       </c>
       <c r="K6" s="141" t="str">
         <f>_xll.qlSimpleQuote(Trigger,J6,,TRUE)</f>
-        <v>EURJump4_SYNTHON_Quote#0001</v>
+        <v>EURJump4_SYNTHON_Quote#0004</v>
       </c>
       <c r="L6" s="141" t="e">
         <f ca="1"/>
@@ -33462,7 +33464,7 @@
       </c>
       <c r="K7" s="141" t="str">
         <f>_xll.qlSimpleQuote(Trigger,J7,,TRUE)</f>
-        <v>EURJump5_SYNTHON_Quote#0001</v>
+        <v>EURJump5_SYNTHON_Quote#0004</v>
       </c>
       <c r="L7" s="141" t="e">
         <f ca="1"/>
@@ -33514,7 +33516,7 @@
       </c>
       <c r="K8" s="141" t="str">
         <f>_xll.qlSimpleQuote(Trigger,J8,,TRUE)</f>
-        <v>EURJump6_SYNTHON_Quote#0001</v>
+        <v>EURJump6_SYNTHON_Quote#0004</v>
       </c>
       <c r="L8" s="141" t="e">
         <f ca="1"/>
@@ -33566,7 +33568,7 @@
       </c>
       <c r="K9" s="141" t="str">
         <f>_xll.qlSimpleQuote(Trigger,J9,,TRUE)</f>
-        <v>EURJump7_SYNTHON_Quote#0001</v>
+        <v>EURJump7_SYNTHON_Quote#0004</v>
       </c>
       <c r="L9" s="141" t="e">
         <f ca="1"/>
@@ -33618,7 +33620,7 @@
       </c>
       <c r="K10" s="141" t="str">
         <f>_xll.qlSimpleQuote(Trigger,J10,,TRUE)</f>
-        <v>EURJump8_SYNTHON_Quote#0001</v>
+        <v>EURJump8_SYNTHON_Quote#0004</v>
       </c>
       <c r="L10" s="141" t="e">
         <f ca="1"/>
@@ -33670,7 +33672,7 @@
       </c>
       <c r="K11" s="141" t="str">
         <f>_xll.qlSimpleQuote(Trigger,J11,,TRUE)</f>
-        <v>EURJump9_SYNTHON_Quote#0001</v>
+        <v>EURJump9_SYNTHON_Quote#0004</v>
       </c>
       <c r="L11" s="141" t="e">
         <f ca="1"/>
@@ -33722,7 +33724,7 @@
       </c>
       <c r="K12" s="141" t="str">
         <f>_xll.qlSimpleQuote(Trigger,J12,,TRUE)</f>
-        <v>EURJump10_SYNTHON_Quote#0001</v>
+        <v>EURJump10_SYNTHON_Quote#0004</v>
       </c>
       <c r="L12" s="141" t="e">
         <f ca="1"/>
@@ -33774,7 +33776,7 @@
       </c>
       <c r="K13" s="141" t="str">
         <f>_xll.qlSimpleQuote(Trigger,J13,,TRUE)</f>
-        <v>EURJump11_SYNTHON_Quote#0001</v>
+        <v>EURJump11_SYNTHON_Quote#0004</v>
       </c>
       <c r="L13" s="141" t="e">
         <f ca="1"/>
@@ -33826,7 +33828,7 @@
       </c>
       <c r="K14" s="141" t="str">
         <f>_xll.qlSimpleQuote(Trigger,J14,,TRUE)</f>
-        <v>EURJump12_SYNTHON_Quote#0001</v>
+        <v>EURJump12_SYNTHON_Quote#0004</v>
       </c>
       <c r="L14" s="141" t="e">
         <f ca="1"/>
@@ -33878,7 +33880,7 @@
       </c>
       <c r="K15" s="142" t="str">
         <f>_xll.qlSimpleQuote(Trigger,J15,,TRUE)</f>
-        <v>EURJump13_SYNTHON_Quote#0001</v>
+        <v>EURJump13_SYNTHON_Quote#0004</v>
       </c>
       <c r="L15" s="142" t="e">
         <f ca="1"/>

</xml_diff>

<commit_message>
implement functions qlRateHelperEarliestDate(), qlRateHelperLatestDate()
</commit_message>
<xml_diff>
--- a/Data2/XLS/EUR/EUR_JumpsQuotesFeedON.xlsx
+++ b/Data2/XLS/EUR/EUR_JumpsQuotesFeedON.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="15300" windowHeight="9570" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="15300" windowHeight="9570" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="General Settings" sheetId="3" r:id="rId1"/>
@@ -1674,11 +1674,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="214941696"/>
-        <c:axId val="214943232"/>
+        <c:axId val="33280384"/>
+        <c:axId val="33281920"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="214941696"/>
+        <c:axId val="33280384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1698,12 +1698,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="214943232"/>
+        <c:crossAx val="33281920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="214943232"/>
+        <c:axId val="33281920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1714,7 +1714,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="214941696"/>
+        <c:crossAx val="33280384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4871,11 +4871,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="221282304"/>
-        <c:axId val="221283840"/>
+        <c:axId val="63541632"/>
+        <c:axId val="63543168"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="221282304"/>
+        <c:axId val="63541632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4895,14 +4895,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="221283840"/>
+        <c:crossAx val="63543168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="221283840"/>
+        <c:axId val="63543168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4913,7 +4913,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="221282304"/>
+        <c:crossAx val="63541632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5045,7 +5045,7 @@
       <sheetData sheetId="0">
         <row r="6">
           <cell r="D6">
-            <v>4</v>
+            <v>1</v>
           </cell>
         </row>
       </sheetData>
@@ -5053,7 +5053,7 @@
       <sheetData sheetId="2">
         <row r="6">
           <cell r="D6" t="str">
-            <v>EUR6M#0004</v>
+            <v>EUR6M#0002</v>
           </cell>
         </row>
       </sheetData>
@@ -5088,7 +5088,7 @@
       <sheetData sheetId="7">
         <row r="6">
           <cell r="D6" t="str">
-            <v>EURTND_Quote#0004</v>
+            <v>EURTND_Quote#0001</v>
           </cell>
         </row>
       </sheetData>
@@ -5542,9 +5542,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5669,7 +5667,7 @@
       </c>
       <c r="I8" s="60">
         <f>[1]!TriggerCounter</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J8" s="58"/>
     </row>
@@ -5689,7 +5687,7 @@
       </c>
       <c r="I9" s="29">
         <f ca="1">_xll.ohTrigger(Contribution!M1)</f>
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="J9" s="4"/>
     </row>
@@ -5842,7 +5840,7 @@
       <c r="B19" s="1"/>
       <c r="C19" s="20" t="e">
         <f ca="1">MAX(_xll.ohPack(Calculation!D5:D129))</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D19" s="73" t="e">
         <f ca="1">_xll.qlYieldTSDiscount(YieldCurve,C19,,Trigger)</f>
@@ -5852,7 +5850,7 @@
       <c r="G19" s="1"/>
       <c r="H19" s="20" t="e">
         <f ca="1">MAX(_xll.ohPack(Calculation!D27:D151))</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="I19" s="73" t="e">
         <f ca="1">_xll.qlYieldTSDiscount($I$14,H19,,Trigger)</f>
@@ -5959,8 +5957,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D1"/>
+    <sheetView showGridLines="0" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -6017,7 +6015,7 @@
       </c>
       <c r="F2" s="77" t="str">
         <f>_xll.qlFraRateHelper(EvaluationDate,"W"&amp;Currency&amp;B2&amp;C2&amp;D2,,,E2,"2d",OvernightIndex)</f>
-        <v>WEURSND#0008</v>
+        <v>WEURSND#0000</v>
       </c>
       <c r="G2" s="78" t="b">
         <v>0</v>
@@ -6028,13 +6026,13 @@
       <c r="I2" s="78">
         <v>1</v>
       </c>
-      <c r="J2" s="79" t="e">
-        <f ca="1">_xll.qlRateHelperEarliestDate($F2)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="K2" s="79" t="e">
-        <f ca="1">_xll.qlRateHelperLatestDate($F2)</f>
-        <v>#NAME?</v>
+      <c r="J2" s="79">
+        <f>_xll.qlRateHelperEarliestDate(Trigger,$F2)</f>
+        <v>42242</v>
+      </c>
+      <c r="K2" s="79">
+        <f>_xll.qlRateHelperLatestDate(Trigger,$F2)</f>
+        <v>42243</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -6058,7 +6056,7 @@
       </c>
       <c r="F3" s="81" t="str">
         <f>_xll.qlDatedOISRateHelper(Trigger,"W"&amp;Currency&amp;B3&amp;C3&amp;D3,,,A3,A4,E3,OvernightIndex)</f>
-        <v>WEURECBOISSEP15#0003</v>
+        <v>WEURECBOISSEP15#0001</v>
       </c>
       <c r="G3" s="82" t="b">
         <f>IF(ISERROR(F3),FALSE,TRUE)</f>
@@ -6070,13 +6068,13 @@
       <c r="I3" s="83">
         <v>5</v>
       </c>
-      <c r="J3" s="84" t="e">
-        <f ca="1">_xll.qlRateHelperEarliestDate($F3)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="K3" s="84" t="e">
-        <f ca="1">_xll.qlRateHelperLatestDate($F3)</f>
-        <v>#NAME?</v>
+      <c r="J3" s="84">
+        <f>_xll.qlRateHelperEarliestDate(Trigger,$F3)</f>
+        <v>42256</v>
+      </c>
+      <c r="K3" s="84">
+        <f>_xll.qlRateHelperLatestDate(Trigger,$F3)</f>
+        <v>42305</v>
       </c>
       <c r="L3" s="94"/>
     </row>
@@ -6101,7 +6099,7 @@
       </c>
       <c r="F4" s="85" t="str">
         <f>_xll.qlDatedOISRateHelper(Trigger,"W"&amp;Currency&amp;B4&amp;C4&amp;D4,,,A4,A5,E4,OvernightIndex)</f>
-        <v>WEURECBOISOCT15#0003</v>
+        <v>WEURECBOISOCT15#0001</v>
       </c>
       <c r="G4" s="82" t="b">
         <f t="shared" ref="G4:G12" si="1">IF(ISERROR(F4),FALSE,TRUE)</f>
@@ -6113,13 +6111,13 @@
       <c r="I4" s="82">
         <v>5</v>
       </c>
-      <c r="J4" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperEarliestDate($F4)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="K4" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperLatestDate($F4)</f>
-        <v>#NAME?</v>
+      <c r="J4" s="86">
+        <f>_xll.qlRateHelperEarliestDate(Trigger,$F4)</f>
+        <v>42305</v>
+      </c>
+      <c r="K4" s="86">
+        <f>_xll.qlRateHelperLatestDate(Trigger,$F4)</f>
+        <v>42347</v>
       </c>
       <c r="L4" s="95"/>
     </row>
@@ -6144,7 +6142,7 @@
       </c>
       <c r="F5" s="85" t="str">
         <f>_xll.qlDatedOISRateHelper(Trigger,"W"&amp;Currency&amp;B5&amp;C5&amp;D5,,,A5,A6,E5,OvernightIndex)</f>
-        <v>WEURECBOISDEC15#0003</v>
+        <v>WEURECBOISDEC15#0001</v>
       </c>
       <c r="G5" s="82" t="b">
         <f t="shared" si="1"/>
@@ -6156,13 +6154,13 @@
       <c r="I5" s="82">
         <v>5</v>
       </c>
-      <c r="J5" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperEarliestDate($F5)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="K5" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperLatestDate($F5)</f>
-        <v>#NAME?</v>
+      <c r="J5" s="86">
+        <f>_xll.qlRateHelperEarliestDate(Trigger,$F5)</f>
+        <v>42347</v>
+      </c>
+      <c r="K5" s="86">
+        <f>_xll.qlRateHelperLatestDate(Trigger,$F5)</f>
+        <v>42395</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -6186,7 +6184,7 @@
       </c>
       <c r="F6" s="85" t="str">
         <f>_xll.qlDatedOISRateHelper(Trigger,"W"&amp;Currency&amp;B6&amp;C6&amp;D6,,,A6,A7,E6,OvernightIndex)</f>
-        <v>WEURECBOISJAN16#0003</v>
+        <v>WEURECBOISJAN16#0001</v>
       </c>
       <c r="G6" s="82" t="b">
         <f t="shared" si="1"/>
@@ -6198,13 +6196,13 @@
       <c r="I6" s="82">
         <v>5</v>
       </c>
-      <c r="J6" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperEarliestDate($F6)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="K6" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperLatestDate($F6)</f>
-        <v>#NAME?</v>
+      <c r="J6" s="86">
+        <f>_xll.qlRateHelperEarliestDate(Trigger,$F6)</f>
+        <v>42395</v>
+      </c>
+      <c r="K6" s="86">
+        <f>_xll.qlRateHelperLatestDate(Trigger,$F6)</f>
+        <v>42445</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -6228,7 +6226,7 @@
       </c>
       <c r="F7" s="85" t="str">
         <f>_xll.qlDatedOISRateHelper(Trigger,"W"&amp;Currency&amp;B7&amp;C7&amp;D7,,,A7,A8,E7,OvernightIndex)</f>
-        <v>WEURECBOISMAR16#0003</v>
+        <v>WEURECBOISMAR16#0001</v>
       </c>
       <c r="G7" s="82" t="b">
         <f t="shared" si="1"/>
@@ -6240,13 +6238,13 @@
       <c r="I7" s="82">
         <v>5</v>
       </c>
-      <c r="J7" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperEarliestDate($F7)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="K7" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperLatestDate($F7)</f>
-        <v>#NAME?</v>
+      <c r="J7" s="86">
+        <f>_xll.qlRateHelperEarliestDate(Trigger,$F7)</f>
+        <v>42445</v>
+      </c>
+      <c r="K7" s="86">
+        <f>_xll.qlRateHelperLatestDate(Trigger,$F7)</f>
+        <v>42487</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -6270,7 +6268,7 @@
       </c>
       <c r="F8" s="85" t="str">
         <f>_xll.qlDatedOISRateHelper(Trigger,"W"&amp;Currency&amp;B8&amp;C8&amp;D8,,,A8,A9,E8,OvernightIndex)</f>
-        <v>WEURECBOISAPR16#0003</v>
+        <v>WEURECBOISAPR16#0001</v>
       </c>
       <c r="G8" s="82" t="b">
         <f t="shared" si="1"/>
@@ -6282,13 +6280,13 @@
       <c r="I8" s="82">
         <v>5</v>
       </c>
-      <c r="J8" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperEarliestDate($F8)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="K8" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperLatestDate($F8)</f>
-        <v>#NAME?</v>
+      <c r="J8" s="86">
+        <f>_xll.qlRateHelperEarliestDate(Trigger,$F8)</f>
+        <v>42487</v>
+      </c>
+      <c r="K8" s="86">
+        <f>_xll.qlRateHelperLatestDate(Trigger,$F8)</f>
+        <v>42529</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -6325,12 +6323,12 @@
         <v>5</v>
       </c>
       <c r="J9" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperEarliestDate($F9)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlRateHelperEarliestDate(Trigger,$F9)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="K9" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperLatestDate($F9)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlRateHelperLatestDate(Trigger,$F9)</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -6367,12 +6365,12 @@
         <v>5</v>
       </c>
       <c r="J10" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperEarliestDate($F10)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlRateHelperEarliestDate(Trigger,$F10)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="K10" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperLatestDate($F10)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlRateHelperLatestDate(Trigger,$F10)</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
@@ -6409,12 +6407,12 @@
         <v>5</v>
       </c>
       <c r="J11" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperEarliestDate($F11)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlRateHelperEarliestDate(Trigger,$F11)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="K11" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperLatestDate($F11)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlRateHelperLatestDate(Trigger,$F11)</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -6451,12 +6449,12 @@
         <v>5</v>
       </c>
       <c r="J12" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperEarliestDate($F12)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlRateHelperEarliestDate(Trigger,$F12)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="K12" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperLatestDate($F12)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlRateHelperLatestDate(Trigger,$F12)</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -6489,12 +6487,12 @@
         <v>7</v>
       </c>
       <c r="J13" s="84" t="e">
-        <f ca="1">_xll.qlRateHelperEarliestDate($F13)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlRateHelperEarliestDate(Trigger,$F13)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="K13" s="84" t="e">
-        <f ca="1">_xll.qlRateHelperLatestDate($F13)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlRateHelperLatestDate(Trigger,$F13)</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -6526,12 +6524,12 @@
         <v>7</v>
       </c>
       <c r="J14" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperEarliestDate($F14)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlRateHelperEarliestDate(Trigger,$F14)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="K14" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperLatestDate($F14)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlRateHelperLatestDate(Trigger,$F14)</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -6563,12 +6561,12 @@
         <v>7</v>
       </c>
       <c r="J15" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperEarliestDate($F15)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlRateHelperEarliestDate(Trigger,$F15)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="K15" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperLatestDate($F15)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlRateHelperLatestDate(Trigger,$F15)</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -6600,12 +6598,12 @@
         <v>7</v>
       </c>
       <c r="J16" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperEarliestDate($F16)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlRateHelperEarliestDate(Trigger,$F16)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="K16" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperLatestDate($F16)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlRateHelperLatestDate(Trigger,$F16)</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -6637,12 +6635,12 @@
         <v>7</v>
       </c>
       <c r="J17" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperEarliestDate($F17)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlRateHelperEarliestDate(Trigger,$F17)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="K17" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperLatestDate($F17)</f>
-        <v>#NAME?</v>
+        <f>_xll.qlRateHelperLatestDate(Trigger,$F17)</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -6672,13 +6670,13 @@
       <c r="I18" s="83">
         <v>1</v>
       </c>
-      <c r="J18" s="84" t="e">
-        <f ca="1">_xll.qlRateHelperEarliestDate($F18)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="K18" s="84" t="e">
-        <f ca="1">_xll.qlRateHelperLatestDate($F18)</f>
-        <v>#NAME?</v>
+      <c r="J18" s="84">
+        <f>_xll.qlRateHelperEarliestDate(Trigger,$F18)</f>
+        <v>42242</v>
+      </c>
+      <c r="K18" s="84">
+        <f>_xll.qlRateHelperLatestDate(Trigger,$F18)</f>
+        <v>42249</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
@@ -6707,13 +6705,13 @@
       <c r="I19" s="82">
         <v>1</v>
       </c>
-      <c r="J19" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperEarliestDate($F19)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="K19" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperLatestDate($F19)</f>
-        <v>#NAME?</v>
+      <c r="J19" s="86">
+        <f>_xll.qlRateHelperEarliestDate(Trigger,$F19)</f>
+        <v>42242</v>
+      </c>
+      <c r="K19" s="86">
+        <f>_xll.qlRateHelperLatestDate(Trigger,$F19)</f>
+        <v>42249</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
@@ -6742,13 +6740,13 @@
       <c r="I20" s="82">
         <v>1</v>
       </c>
-      <c r="J20" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperEarliestDate($F20)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="K20" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperLatestDate($F20)</f>
-        <v>#NAME?</v>
+      <c r="J20" s="86">
+        <f>_xll.qlRateHelperEarliestDate(Trigger,$F20)</f>
+        <v>42242</v>
+      </c>
+      <c r="K20" s="86">
+        <f>_xll.qlRateHelperLatestDate(Trigger,$F20)</f>
+        <v>42249</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
@@ -6777,13 +6775,13 @@
       <c r="I21" s="82">
         <v>1</v>
       </c>
-      <c r="J21" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperEarliestDate($F21)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="K21" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperLatestDate($F21)</f>
-        <v>#NAME?</v>
+      <c r="J21" s="86">
+        <f>_xll.qlRateHelperEarliestDate(Trigger,$F21)</f>
+        <v>42242</v>
+      </c>
+      <c r="K21" s="86">
+        <f>_xll.qlRateHelperLatestDate(Trigger,$F21)</f>
+        <v>42249</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
@@ -6812,13 +6810,13 @@
       <c r="I22" s="82">
         <v>1</v>
       </c>
-      <c r="J22" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperEarliestDate($F22)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="K22" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperLatestDate($F22)</f>
-        <v>#NAME?</v>
+      <c r="J22" s="86">
+        <f>_xll.qlRateHelperEarliestDate(Trigger,$F22)</f>
+        <v>42242</v>
+      </c>
+      <c r="K22" s="86">
+        <f>_xll.qlRateHelperLatestDate(Trigger,$F22)</f>
+        <v>42249</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
@@ -6847,13 +6845,13 @@
       <c r="I23" s="82">
         <v>1</v>
       </c>
-      <c r="J23" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperEarliestDate($F23)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="K23" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperLatestDate($F23)</f>
-        <v>#NAME?</v>
+      <c r="J23" s="86">
+        <f>_xll.qlRateHelperEarliestDate(Trigger,$F23)</f>
+        <v>42242</v>
+      </c>
+      <c r="K23" s="86">
+        <f>_xll.qlRateHelperLatestDate(Trigger,$F23)</f>
+        <v>42249</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
@@ -6882,13 +6880,13 @@
       <c r="I24" s="82">
         <v>1</v>
       </c>
-      <c r="J24" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperEarliestDate($F24)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="K24" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperLatestDate($F24)</f>
-        <v>#NAME?</v>
+      <c r="J24" s="86">
+        <f>_xll.qlRateHelperEarliestDate(Trigger,$F24)</f>
+        <v>42242</v>
+      </c>
+      <c r="K24" s="86">
+        <f>_xll.qlRateHelperLatestDate(Trigger,$F24)</f>
+        <v>42249</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
@@ -6917,13 +6915,13 @@
       <c r="I25" s="82">
         <v>1</v>
       </c>
-      <c r="J25" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperEarliestDate($F25)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="K25" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperLatestDate($F25)</f>
-        <v>#NAME?</v>
+      <c r="J25" s="86">
+        <f>_xll.qlRateHelperEarliestDate(Trigger,$F25)</f>
+        <v>42242</v>
+      </c>
+      <c r="K25" s="86">
+        <f>_xll.qlRateHelperLatestDate(Trigger,$F25)</f>
+        <v>42249</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
@@ -6952,13 +6950,13 @@
       <c r="I26" s="82">
         <v>1</v>
       </c>
-      <c r="J26" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperEarliestDate($F26)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="K26" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperLatestDate($F26)</f>
-        <v>#NAME?</v>
+      <c r="J26" s="86">
+        <f>_xll.qlRateHelperEarliestDate(Trigger,$F26)</f>
+        <v>42242</v>
+      </c>
+      <c r="K26" s="86">
+        <f>_xll.qlRateHelperLatestDate(Trigger,$F26)</f>
+        <v>42249</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
@@ -6987,13 +6985,13 @@
       <c r="I27" s="82">
         <v>1</v>
       </c>
-      <c r="J27" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperEarliestDate($F27)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="K27" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperLatestDate($F27)</f>
-        <v>#NAME?</v>
+      <c r="J27" s="86">
+        <f>_xll.qlRateHelperEarliestDate(Trigger,$F27)</f>
+        <v>42242</v>
+      </c>
+      <c r="K27" s="86">
+        <f>_xll.qlRateHelperLatestDate(Trigger,$F27)</f>
+        <v>42249</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
@@ -7022,13 +7020,13 @@
       <c r="I28" s="82">
         <v>1</v>
       </c>
-      <c r="J28" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperEarliestDate($F28)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="K28" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperLatestDate($F28)</f>
-        <v>#NAME?</v>
+      <c r="J28" s="86">
+        <f>_xll.qlRateHelperEarliestDate(Trigger,$F28)</f>
+        <v>42242</v>
+      </c>
+      <c r="K28" s="86">
+        <f>_xll.qlRateHelperLatestDate(Trigger,$F28)</f>
+        <v>42249</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
@@ -7057,13 +7055,13 @@
       <c r="I29" s="82">
         <v>1</v>
       </c>
-      <c r="J29" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperEarliestDate($F29)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="K29" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperLatestDate($F29)</f>
-        <v>#NAME?</v>
+      <c r="J29" s="86">
+        <f>_xll.qlRateHelperEarliestDate(Trigger,$F29)</f>
+        <v>42242</v>
+      </c>
+      <c r="K29" s="86">
+        <f>_xll.qlRateHelperLatestDate(Trigger,$F29)</f>
+        <v>42249</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
@@ -7092,13 +7090,13 @@
       <c r="I30" s="82">
         <v>1</v>
       </c>
-      <c r="J30" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperEarliestDate($F30)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="K30" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperLatestDate($F30)</f>
-        <v>#NAME?</v>
+      <c r="J30" s="86">
+        <f>_xll.qlRateHelperEarliestDate(Trigger,$F30)</f>
+        <v>42242</v>
+      </c>
+      <c r="K30" s="86">
+        <f>_xll.qlRateHelperLatestDate(Trigger,$F30)</f>
+        <v>42249</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
@@ -7127,13 +7125,13 @@
       <c r="I31" s="82">
         <v>1</v>
       </c>
-      <c r="J31" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperEarliestDate($F31)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="K31" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperLatestDate($F31)</f>
-        <v>#NAME?</v>
+      <c r="J31" s="86">
+        <f>_xll.qlRateHelperEarliestDate(Trigger,$F31)</f>
+        <v>42242</v>
+      </c>
+      <c r="K31" s="86">
+        <f>_xll.qlRateHelperLatestDate(Trigger,$F31)</f>
+        <v>42249</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
@@ -7162,13 +7160,13 @@
       <c r="I32" s="82">
         <v>1</v>
       </c>
-      <c r="J32" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperEarliestDate($F32)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="K32" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperLatestDate($F32)</f>
-        <v>#NAME?</v>
+      <c r="J32" s="86">
+        <f>_xll.qlRateHelperEarliestDate(Trigger,$F32)</f>
+        <v>42242</v>
+      </c>
+      <c r="K32" s="86">
+        <f>_xll.qlRateHelperLatestDate(Trigger,$F32)</f>
+        <v>42249</v>
       </c>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.2">
@@ -7197,13 +7195,13 @@
       <c r="I33" s="82">
         <v>1</v>
       </c>
-      <c r="J33" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperEarliestDate($F33)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="K33" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperLatestDate($F33)</f>
-        <v>#NAME?</v>
+      <c r="J33" s="86">
+        <f>_xll.qlRateHelperEarliestDate(Trigger,$F33)</f>
+        <v>42242</v>
+      </c>
+      <c r="K33" s="86">
+        <f>_xll.qlRateHelperLatestDate(Trigger,$F33)</f>
+        <v>42249</v>
       </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.2">
@@ -7232,13 +7230,13 @@
       <c r="I34" s="82">
         <v>1</v>
       </c>
-      <c r="J34" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperEarliestDate($F34)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="K34" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperLatestDate($F34)</f>
-        <v>#NAME?</v>
+      <c r="J34" s="86">
+        <f>_xll.qlRateHelperEarliestDate(Trigger,$F34)</f>
+        <v>42242</v>
+      </c>
+      <c r="K34" s="86">
+        <f>_xll.qlRateHelperLatestDate(Trigger,$F34)</f>
+        <v>42249</v>
       </c>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.2">
@@ -7267,13 +7265,13 @@
       <c r="I35" s="82">
         <v>1</v>
       </c>
-      <c r="J35" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperEarliestDate($F35)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="K35" s="86" t="e">
-        <f ca="1">_xll.qlRateHelperLatestDate($F35)</f>
-        <v>#NAME?</v>
+      <c r="J35" s="86">
+        <f>_xll.qlRateHelperEarliestDate(Trigger,$F35)</f>
+        <v>42242</v>
+      </c>
+      <c r="K35" s="86">
+        <f>_xll.qlRateHelperLatestDate(Trigger,$F35)</f>
+        <v>42249</v>
       </c>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.2">
@@ -7302,13 +7300,13 @@
       <c r="I36" s="91">
         <v>1</v>
       </c>
-      <c r="J36" s="92" t="e">
-        <f ca="1">_xll.qlRateHelperEarliestDate($F36)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="K36" s="92" t="e">
-        <f ca="1">_xll.qlRateHelperLatestDate($F36)</f>
-        <v>#NAME?</v>
+      <c r="J36" s="92">
+        <f>_xll.qlRateHelperEarliestDate(Trigger,$F36)</f>
+        <v>42242</v>
+      </c>
+      <c r="K36" s="92">
+        <f>_xll.qlRateHelperLatestDate(Trigger,$F36)</f>
+        <v>42249</v>
       </c>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.2">
@@ -7324,35 +7322,35 @@
     <row r="38" spans="2:11" x14ac:dyDescent="0.2">
       <c r="D38" s="93">
         <f>_xll.ohTrigger(RateHelpers)</f>
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="E38" s="93">
         <f>_xll.ohTrigger(RateHelpers)</f>
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="F38" s="93">
         <f>_xll.ohTrigger(RateHelpers)</f>
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="G38" s="93">
         <f>_xll.ohTrigger(RateHelpers)</f>
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="H38" s="93">
         <f>_xll.ohTrigger(RateHelpers)</f>
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="I38" s="93">
         <f>_xll.ohTrigger(RateHelpers)</f>
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="J38" s="93">
         <f>_xll.ohTrigger(RateHelpers)</f>
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="K38" s="93">
         <f>_xll.ohTrigger(RateHelpers)</f>
-        <v>13</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -7372,20 +7370,20 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:BK130"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="11" topLeftCell="L1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N16" sqref="N16"/>
+      <selection pane="topRight" activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.140625" style="98" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="2" max="2" width="10" style="98" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="3" max="4" width="17.28515625" style="98" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="5" width="2.7109375" style="93" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="6" width="10" style="93" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="7" style="93" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="2.7109375" style="93" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="16.140625" style="98" customWidth="1" outlineLevel="1"/>
+    <col min="2" max="2" width="10" style="98" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="4" width="17.28515625" style="98" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="2.7109375" style="93" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="10" style="93" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="7" style="93" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="2.7109375" style="93" customWidth="1"/>
     <col min="9" max="9" width="17.28515625" style="93" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" style="93" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.28515625" style="93" bestFit="1" customWidth="1"/>
@@ -8006,11 +8004,11 @@
       </c>
       <c r="C5" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A5)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D5" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A5)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F5" s="103" t="e">
         <f t="shared" ref="F5:F30" ca="1" si="0">IF(ISERROR(D5),NA(),(D5-D4)/2+D4)</f>
@@ -8031,7 +8029,7 @@
       </c>
       <c r="K5" s="113" t="e">
         <f ca="1">D5</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L5" s="94"/>
       <c r="M5" s="85" t="b">
@@ -8208,11 +8206,11 @@
       </c>
       <c r="C6" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A6)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D6" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A6)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F6" s="103" t="e">
         <f t="shared" ca="1" si="0"/>
@@ -8233,7 +8231,7 @@
       </c>
       <c r="K6" s="113" t="e">
         <f t="shared" ref="K6:K69" ca="1" si="3">D6</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L6" s="94"/>
       <c r="M6" s="85" t="b">
@@ -8410,11 +8408,11 @@
       </c>
       <c r="C7" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A7)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D7" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A7)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F7" s="103" t="e">
         <f t="shared" ca="1" si="0"/>
@@ -8434,7 +8432,7 @@
       </c>
       <c r="K7" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L7" s="94"/>
       <c r="M7" s="85" t="b">
@@ -8611,11 +8609,11 @@
       </c>
       <c r="C8" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A8)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D8" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A8)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F8" s="103" t="e">
         <f t="shared" ca="1" si="0"/>
@@ -8635,7 +8633,7 @@
       </c>
       <c r="K8" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L8" s="94"/>
       <c r="M8" s="85" t="b">
@@ -8812,11 +8810,11 @@
       </c>
       <c r="C9" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A9)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D9" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A9)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F9" s="103" t="e">
         <f t="shared" ca="1" si="0"/>
@@ -8836,7 +8834,7 @@
       </c>
       <c r="K9" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L9" s="94"/>
       <c r="M9" s="85" t="b">
@@ -9013,11 +9011,11 @@
       </c>
       <c r="C10" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A10)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D10" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A10)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F10" s="103" t="e">
         <f t="shared" ca="1" si="0"/>
@@ -9037,7 +9035,7 @@
       </c>
       <c r="K10" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L10" s="94"/>
       <c r="M10" s="85" t="b">
@@ -9214,11 +9212,11 @@
       </c>
       <c r="C11" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A11)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D11" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A11)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F11" s="103" t="e">
         <f t="shared" ca="1" si="0"/>
@@ -9238,7 +9236,7 @@
       </c>
       <c r="K11" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L11" s="94"/>
       <c r="M11" s="85" t="b">
@@ -9415,11 +9413,11 @@
       </c>
       <c r="C12" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A12)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D12" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A12)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F12" s="103" t="e">
         <f t="shared" ca="1" si="0"/>
@@ -9439,7 +9437,7 @@
       </c>
       <c r="K12" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L12" s="94"/>
       <c r="M12" s="85" t="b">
@@ -9616,11 +9614,11 @@
       </c>
       <c r="C13" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A13)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D13" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A13)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F13" s="103" t="e">
         <f t="shared" ca="1" si="0"/>
@@ -9640,7 +9638,7 @@
       </c>
       <c r="K13" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L13" s="94"/>
       <c r="M13" s="85" t="b">
@@ -9817,11 +9815,11 @@
       </c>
       <c r="C14" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A14)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D14" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A14)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F14" s="103" t="e">
         <f t="shared" ca="1" si="0"/>
@@ -9841,7 +9839,7 @@
       </c>
       <c r="K14" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L14" s="94"/>
       <c r="M14" s="85" t="b">
@@ -10018,11 +10016,11 @@
       </c>
       <c r="C15" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A15)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D15" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A15)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F15" s="103" t="e">
         <f t="shared" ca="1" si="0"/>
@@ -10042,7 +10040,7 @@
       </c>
       <c r="K15" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L15" s="94"/>
       <c r="M15" s="85" t="b">
@@ -10219,11 +10217,11 @@
       </c>
       <c r="C16" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A16)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D16" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A16)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F16" s="103" t="e">
         <f t="shared" ca="1" si="0"/>
@@ -10243,7 +10241,7 @@
       </c>
       <c r="K16" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L16" s="94"/>
       <c r="M16" s="85" t="b">
@@ -10420,11 +10418,11 @@
       </c>
       <c r="C17" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A17)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D17" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A17)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F17" s="103" t="e">
         <f t="shared" ca="1" si="0"/>
@@ -10444,7 +10442,7 @@
       </c>
       <c r="K17" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L17" s="94"/>
       <c r="M17" s="85" t="b">
@@ -10621,11 +10619,11 @@
       </c>
       <c r="C18" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A18)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D18" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A18)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F18" s="103" t="e">
         <f t="shared" ca="1" si="0"/>
@@ -10645,7 +10643,7 @@
       </c>
       <c r="K18" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L18" s="94"/>
       <c r="M18" s="85" t="b">
@@ -10822,11 +10820,11 @@
       </c>
       <c r="C19" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A19)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D19" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A19)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F19" s="103" t="e">
         <f t="shared" ca="1" si="0"/>
@@ -10846,7 +10844,7 @@
       </c>
       <c r="K19" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L19" s="94"/>
       <c r="M19" s="85" t="b">
@@ -11023,11 +11021,11 @@
       </c>
       <c r="C20" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A20)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D20" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A20)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F20" s="103" t="e">
         <f t="shared" ca="1" si="0"/>
@@ -11047,7 +11045,7 @@
       </c>
       <c r="K20" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L20" s="94"/>
       <c r="M20" s="85" t="b">
@@ -11224,11 +11222,11 @@
       </c>
       <c r="C21" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A21)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D21" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A21)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F21" s="103" t="e">
         <f t="shared" ca="1" si="0"/>
@@ -11248,7 +11246,7 @@
       </c>
       <c r="K21" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L21" s="94"/>
       <c r="M21" s="85" t="b">
@@ -11425,11 +11423,11 @@
       </c>
       <c r="C22" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A22)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D22" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A22)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F22" s="103" t="e">
         <f t="shared" ca="1" si="0"/>
@@ -11449,7 +11447,7 @@
       </c>
       <c r="K22" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L22" s="94"/>
       <c r="M22" s="85" t="b">
@@ -11626,11 +11624,11 @@
       </c>
       <c r="C23" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A23)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D23" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A23)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F23" s="103" t="e">
         <f t="shared" ca="1" si="0"/>
@@ -11650,7 +11648,7 @@
       </c>
       <c r="K23" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L23" s="94"/>
       <c r="M23" s="85" t="b">
@@ -11827,11 +11825,11 @@
       </c>
       <c r="C24" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A24)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D24" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A24)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F24" s="103" t="e">
         <f t="shared" ca="1" si="0"/>
@@ -11851,7 +11849,7 @@
       </c>
       <c r="K24" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L24" s="94"/>
       <c r="M24" s="85" t="b">
@@ -12028,11 +12026,11 @@
       </c>
       <c r="C25" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A25)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D25" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A25)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F25" s="103" t="e">
         <f t="shared" ca="1" si="0"/>
@@ -12052,7 +12050,7 @@
       </c>
       <c r="K25" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L25" s="94"/>
       <c r="M25" s="85" t="b">
@@ -12229,11 +12227,11 @@
       </c>
       <c r="C26" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A26)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D26" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A26)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F26" s="103" t="e">
         <f t="shared" ca="1" si="0"/>
@@ -12253,7 +12251,7 @@
       </c>
       <c r="K26" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L26" s="94"/>
       <c r="M26" s="85" t="b">
@@ -12430,11 +12428,11 @@
       </c>
       <c r="C27" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A27)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D27" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A27)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F27" s="103" t="e">
         <f t="shared" ca="1" si="0"/>
@@ -12454,7 +12452,7 @@
       </c>
       <c r="K27" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L27" s="94"/>
       <c r="M27" s="85" t="b">
@@ -12631,11 +12629,11 @@
       </c>
       <c r="C28" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A28)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D28" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A28)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F28" s="103" t="e">
         <f t="shared" ca="1" si="0"/>
@@ -12655,7 +12653,7 @@
       </c>
       <c r="K28" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L28" s="94"/>
       <c r="M28" s="85" t="b">
@@ -12832,11 +12830,11 @@
       </c>
       <c r="C29" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A29)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D29" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A29)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F29" s="103" t="e">
         <f t="shared" ca="1" si="0"/>
@@ -12856,7 +12854,7 @@
       </c>
       <c r="K29" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L29" s="94"/>
       <c r="M29" s="85" t="b">
@@ -13033,11 +13031,11 @@
       </c>
       <c r="C30" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A30)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D30" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A30)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F30" s="103" t="e">
         <f t="shared" ca="1" si="0"/>
@@ -13057,7 +13055,7 @@
       </c>
       <c r="K30" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L30" s="94"/>
       <c r="M30" s="85" t="b">
@@ -13234,11 +13232,11 @@
       </c>
       <c r="C31" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A31)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D31" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A31)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F31" s="103" t="e">
         <f t="shared" ref="F31:F94" ca="1" si="4">IF(ISERROR(D31),NA(),(D31-D30)/2+D30)</f>
@@ -13258,7 +13256,7 @@
       </c>
       <c r="K31" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L31" s="125"/>
       <c r="M31" s="85" t="b">
@@ -13435,11 +13433,11 @@
       </c>
       <c r="C32" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A32)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D32" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A32)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F32" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -13459,7 +13457,7 @@
       </c>
       <c r="K32" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L32" s="125"/>
       <c r="M32" s="85" t="b">
@@ -13636,11 +13634,11 @@
       </c>
       <c r="C33" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A33)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D33" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A33)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F33" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -13660,7 +13658,7 @@
       </c>
       <c r="K33" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L33" s="125"/>
       <c r="M33" s="85" t="b">
@@ -13837,11 +13835,11 @@
       </c>
       <c r="C34" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A34)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D34" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A34)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F34" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -13861,7 +13859,7 @@
       </c>
       <c r="K34" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L34" s="125"/>
       <c r="M34" s="85" t="b">
@@ -14038,11 +14036,11 @@
       </c>
       <c r="C35" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A35)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D35" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A35)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F35" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -14062,7 +14060,7 @@
       </c>
       <c r="K35" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L35" s="125"/>
       <c r="M35" s="85" t="b">
@@ -14239,11 +14237,11 @@
       </c>
       <c r="C36" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A36)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D36" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A36)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F36" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -14263,7 +14261,7 @@
       </c>
       <c r="K36" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L36" s="125"/>
       <c r="M36" s="85" t="b">
@@ -14440,11 +14438,11 @@
       </c>
       <c r="C37" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A37)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D37" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A37)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F37" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -14464,7 +14462,7 @@
       </c>
       <c r="K37" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L37" s="125"/>
       <c r="M37" s="85" t="b">
@@ -14641,11 +14639,11 @@
       </c>
       <c r="C38" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A38)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D38" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A38)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F38" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -14665,7 +14663,7 @@
       </c>
       <c r="K38" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L38" s="125"/>
       <c r="M38" s="85" t="b">
@@ -14842,11 +14840,11 @@
       </c>
       <c r="C39" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A39)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D39" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A39)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F39" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -14866,7 +14864,7 @@
       </c>
       <c r="K39" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L39" s="125"/>
       <c r="M39" s="85" t="b">
@@ -15043,11 +15041,11 @@
       </c>
       <c r="C40" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A40)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D40" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A40)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F40" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -15067,7 +15065,7 @@
       </c>
       <c r="K40" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L40" s="125"/>
       <c r="M40" s="85" t="b">
@@ -15244,11 +15242,11 @@
       </c>
       <c r="C41" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A41)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D41" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A41)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F41" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -15268,7 +15266,7 @@
       </c>
       <c r="K41" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L41" s="125"/>
       <c r="M41" s="85" t="b">
@@ -15445,11 +15443,11 @@
       </c>
       <c r="C42" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A42)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D42" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A42)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F42" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -15469,7 +15467,7 @@
       </c>
       <c r="K42" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L42" s="125"/>
       <c r="M42" s="85" t="b">
@@ -15646,11 +15644,11 @@
       </c>
       <c r="C43" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A43)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D43" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A43)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F43" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -15670,7 +15668,7 @@
       </c>
       <c r="K43" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L43" s="125"/>
       <c r="M43" s="85" t="b">
@@ -15847,11 +15845,11 @@
       </c>
       <c r="C44" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A44)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D44" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A44)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F44" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -15871,7 +15869,7 @@
       </c>
       <c r="K44" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L44" s="125"/>
       <c r="M44" s="85" t="b">
@@ -16048,11 +16046,11 @@
       </c>
       <c r="C45" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A45)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D45" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A45)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F45" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -16072,7 +16070,7 @@
       </c>
       <c r="K45" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L45" s="125"/>
       <c r="M45" s="85" t="b">
@@ -16249,11 +16247,11 @@
       </c>
       <c r="C46" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A46)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D46" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A46)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F46" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -16273,7 +16271,7 @@
       </c>
       <c r="K46" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L46" s="125"/>
       <c r="M46" s="85" t="b">
@@ -16450,11 +16448,11 @@
       </c>
       <c r="C47" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A47)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D47" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A47)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F47" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -16474,7 +16472,7 @@
       </c>
       <c r="K47" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L47" s="125"/>
       <c r="M47" s="85" t="b">
@@ -16651,11 +16649,11 @@
       </c>
       <c r="C48" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A48)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D48" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A48)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F48" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -16675,7 +16673,7 @@
       </c>
       <c r="K48" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L48" s="125"/>
       <c r="M48" s="85" t="b">
@@ -16852,11 +16850,11 @@
       </c>
       <c r="C49" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A49)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D49" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A49)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F49" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -16876,7 +16874,7 @@
       </c>
       <c r="K49" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L49" s="125"/>
       <c r="M49" s="85" t="b">
@@ -17053,11 +17051,11 @@
       </c>
       <c r="C50" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A50)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D50" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A50)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F50" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -17077,7 +17075,7 @@
       </c>
       <c r="K50" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L50" s="125"/>
       <c r="M50" s="85" t="b">
@@ -17254,11 +17252,11 @@
       </c>
       <c r="C51" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A51)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D51" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A51)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F51" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -17278,7 +17276,7 @@
       </c>
       <c r="K51" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L51" s="125"/>
       <c r="M51" s="85" t="b">
@@ -17455,11 +17453,11 @@
       </c>
       <c r="C52" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A52)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D52" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A52)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F52" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -17479,7 +17477,7 @@
       </c>
       <c r="K52" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L52" s="125"/>
       <c r="M52" s="85" t="b">
@@ -17656,11 +17654,11 @@
       </c>
       <c r="C53" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A53)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D53" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A53)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F53" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -17680,7 +17678,7 @@
       </c>
       <c r="K53" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L53" s="125"/>
       <c r="M53" s="85" t="b">
@@ -17857,11 +17855,11 @@
       </c>
       <c r="C54" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A54)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D54" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A54)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F54" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -17881,7 +17879,7 @@
       </c>
       <c r="K54" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L54" s="125"/>
       <c r="M54" s="85" t="b">
@@ -18058,11 +18056,11 @@
       </c>
       <c r="C55" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A55)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D55" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A55)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F55" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -18082,7 +18080,7 @@
       </c>
       <c r="K55" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L55" s="125"/>
       <c r="M55" s="85" t="b">
@@ -18259,11 +18257,11 @@
       </c>
       <c r="C56" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A56)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D56" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A56)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F56" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -18283,7 +18281,7 @@
       </c>
       <c r="K56" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L56" s="125"/>
       <c r="M56" s="85" t="b">
@@ -18460,11 +18458,11 @@
       </c>
       <c r="C57" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A57)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D57" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A57)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F57" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -18484,7 +18482,7 @@
       </c>
       <c r="K57" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L57" s="125"/>
       <c r="M57" s="85" t="b">
@@ -18661,11 +18659,11 @@
       </c>
       <c r="C58" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A58)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D58" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A58)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F58" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -18685,7 +18683,7 @@
       </c>
       <c r="K58" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L58" s="125"/>
       <c r="M58" s="85" t="b">
@@ -18862,11 +18860,11 @@
       </c>
       <c r="C59" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A59)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D59" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A59)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F59" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -18886,7 +18884,7 @@
       </c>
       <c r="K59" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L59" s="125"/>
       <c r="M59" s="85" t="b">
@@ -19063,11 +19061,11 @@
       </c>
       <c r="C60" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A60)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D60" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A60)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F60" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -19087,7 +19085,7 @@
       </c>
       <c r="K60" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L60" s="125"/>
       <c r="M60" s="85" t="b">
@@ -19264,11 +19262,11 @@
       </c>
       <c r="C61" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A61)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D61" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A61)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F61" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -19288,7 +19286,7 @@
       </c>
       <c r="K61" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L61" s="125"/>
       <c r="M61" s="85" t="b">
@@ -19465,11 +19463,11 @@
       </c>
       <c r="C62" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A62)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D62" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A62)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F62" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -19489,7 +19487,7 @@
       </c>
       <c r="K62" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L62" s="125"/>
       <c r="M62" s="85" t="b">
@@ -19666,11 +19664,11 @@
       </c>
       <c r="C63" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A63)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D63" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A63)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F63" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -19690,7 +19688,7 @@
       </c>
       <c r="K63" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L63" s="125"/>
       <c r="M63" s="85" t="b">
@@ -19867,11 +19865,11 @@
       </c>
       <c r="C64" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A64)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D64" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A64)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F64" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -19891,7 +19889,7 @@
       </c>
       <c r="K64" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L64" s="125"/>
       <c r="M64" s="85" t="b">
@@ -20068,11 +20066,11 @@
       </c>
       <c r="C65" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A65)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D65" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A65)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F65" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -20092,7 +20090,7 @@
       </c>
       <c r="K65" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L65" s="125"/>
       <c r="M65" s="85" t="b">
@@ -20269,11 +20267,11 @@
       </c>
       <c r="C66" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A66)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D66" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A66)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F66" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -20293,7 +20291,7 @@
       </c>
       <c r="K66" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L66" s="125"/>
       <c r="M66" s="85" t="b">
@@ -20470,11 +20468,11 @@
       </c>
       <c r="C67" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A67)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D67" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A67)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F67" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -20494,7 +20492,7 @@
       </c>
       <c r="K67" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L67" s="125"/>
       <c r="M67" s="85" t="b">
@@ -20671,11 +20669,11 @@
       </c>
       <c r="C68" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A68)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D68" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A68)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F68" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -20695,7 +20693,7 @@
       </c>
       <c r="K68" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L68" s="125"/>
       <c r="M68" s="85" t="b">
@@ -20872,11 +20870,11 @@
       </c>
       <c r="C69" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A69)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D69" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A69)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F69" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -20896,7 +20894,7 @@
       </c>
       <c r="K69" s="113" t="e">
         <f t="shared" ca="1" si="3"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L69" s="125"/>
       <c r="M69" s="85" t="b">
@@ -21073,11 +21071,11 @@
       </c>
       <c r="C70" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A70)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D70" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A70)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F70" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -21097,7 +21095,7 @@
       </c>
       <c r="K70" s="113" t="e">
         <f t="shared" ref="K70:K129" ca="1" si="8">D70</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L70" s="125"/>
       <c r="M70" s="85" t="b">
@@ -21274,11 +21272,11 @@
       </c>
       <c r="C71" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A71)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D71" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A71)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F71" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -21298,7 +21296,7 @@
       </c>
       <c r="K71" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L71" s="125"/>
       <c r="M71" s="85" t="b">
@@ -21475,11 +21473,11 @@
       </c>
       <c r="C72" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A72)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D72" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A72)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F72" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -21499,7 +21497,7 @@
       </c>
       <c r="K72" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L72" s="125"/>
       <c r="M72" s="85" t="b">
@@ -21676,11 +21674,11 @@
       </c>
       <c r="C73" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A73)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D73" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A73)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F73" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -21700,7 +21698,7 @@
       </c>
       <c r="K73" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L73" s="125"/>
       <c r="M73" s="85" t="b">
@@ -21877,11 +21875,11 @@
       </c>
       <c r="C74" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A74)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D74" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A74)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F74" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -21901,7 +21899,7 @@
       </c>
       <c r="K74" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L74" s="125"/>
       <c r="M74" s="85" t="b">
@@ -22078,11 +22076,11 @@
       </c>
       <c r="C75" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A75)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D75" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A75)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F75" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -22102,7 +22100,7 @@
       </c>
       <c r="K75" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L75" s="125"/>
       <c r="M75" s="85" t="b">
@@ -22279,11 +22277,11 @@
       </c>
       <c r="C76" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A76)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D76" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A76)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F76" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -22303,7 +22301,7 @@
       </c>
       <c r="K76" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L76" s="125"/>
       <c r="M76" s="85" t="b">
@@ -22480,11 +22478,11 @@
       </c>
       <c r="C77" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A77)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D77" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A77)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F77" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -22504,7 +22502,7 @@
       </c>
       <c r="K77" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L77" s="125"/>
       <c r="M77" s="85" t="b">
@@ -22681,11 +22679,11 @@
       </c>
       <c r="C78" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A78)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D78" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A78)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F78" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -22705,7 +22703,7 @@
       </c>
       <c r="K78" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L78" s="125"/>
       <c r="M78" s="85" t="b">
@@ -22882,11 +22880,11 @@
       </c>
       <c r="C79" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A79)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D79" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A79)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F79" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -22906,7 +22904,7 @@
       </c>
       <c r="K79" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L79" s="125"/>
       <c r="M79" s="85" t="b">
@@ -23083,11 +23081,11 @@
       </c>
       <c r="C80" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A80)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D80" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A80)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F80" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -23107,7 +23105,7 @@
       </c>
       <c r="K80" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L80" s="125"/>
       <c r="M80" s="85" t="b">
@@ -23284,11 +23282,11 @@
       </c>
       <c r="C81" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A81)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D81" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A81)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F81" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -23308,7 +23306,7 @@
       </c>
       <c r="K81" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L81" s="125"/>
       <c r="M81" s="85" t="b">
@@ -23485,11 +23483,11 @@
       </c>
       <c r="C82" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A82)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D82" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A82)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F82" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -23509,7 +23507,7 @@
       </c>
       <c r="K82" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L82" s="125"/>
       <c r="M82" s="85" t="b">
@@ -23686,11 +23684,11 @@
       </c>
       <c r="C83" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A83)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D83" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A83)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F83" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -23710,7 +23708,7 @@
       </c>
       <c r="K83" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L83" s="125"/>
       <c r="M83" s="85" t="b">
@@ -23887,11 +23885,11 @@
       </c>
       <c r="C84" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A84)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D84" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A84)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F84" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -23911,7 +23909,7 @@
       </c>
       <c r="K84" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L84" s="125"/>
       <c r="M84" s="85" t="b">
@@ -24088,11 +24086,11 @@
       </c>
       <c r="C85" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A85)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D85" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A85)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F85" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -24112,7 +24110,7 @@
       </c>
       <c r="K85" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L85" s="125"/>
       <c r="M85" s="85" t="b">
@@ -24289,11 +24287,11 @@
       </c>
       <c r="C86" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A86)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D86" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A86)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F86" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -24313,7 +24311,7 @@
       </c>
       <c r="K86" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L86" s="125"/>
       <c r="M86" s="85" t="b">
@@ -24490,11 +24488,11 @@
       </c>
       <c r="C87" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A87)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D87" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A87)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F87" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -24514,7 +24512,7 @@
       </c>
       <c r="K87" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L87" s="125"/>
       <c r="M87" s="85" t="b">
@@ -24691,11 +24689,11 @@
       </c>
       <c r="C88" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A88)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D88" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A88)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F88" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -24715,7 +24713,7 @@
       </c>
       <c r="K88" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L88" s="125"/>
       <c r="M88" s="85" t="b">
@@ -24892,11 +24890,11 @@
       </c>
       <c r="C89" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A89)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D89" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A89)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F89" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -24916,7 +24914,7 @@
       </c>
       <c r="K89" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L89" s="125"/>
       <c r="M89" s="85" t="b">
@@ -25093,11 +25091,11 @@
       </c>
       <c r="C90" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A90)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D90" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A90)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F90" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -25117,7 +25115,7 @@
       </c>
       <c r="K90" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L90" s="125"/>
       <c r="M90" s="85" t="b">
@@ -25294,11 +25292,11 @@
       </c>
       <c r="C91" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A91)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D91" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A91)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F91" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -25318,7 +25316,7 @@
       </c>
       <c r="K91" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L91" s="125"/>
       <c r="M91" s="85" t="b">
@@ -25495,11 +25493,11 @@
       </c>
       <c r="C92" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A92)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D92" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A92)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F92" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -25519,7 +25517,7 @@
       </c>
       <c r="K92" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L92" s="125"/>
       <c r="M92" s="85" t="b">
@@ -25696,11 +25694,11 @@
       </c>
       <c r="C93" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A93)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D93" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A93)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F93" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -25720,7 +25718,7 @@
       </c>
       <c r="K93" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L93" s="125"/>
       <c r="M93" s="85" t="b">
@@ -25897,11 +25895,11 @@
       </c>
       <c r="C94" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A94)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D94" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A94)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F94" s="103" t="e">
         <f t="shared" ca="1" si="4"/>
@@ -25921,7 +25919,7 @@
       </c>
       <c r="K94" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L94" s="125"/>
       <c r="M94" s="85" t="b">
@@ -26098,11 +26096,11 @@
       </c>
       <c r="C95" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A95)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D95" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A95)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F95" s="103" t="e">
         <f t="shared" ref="F95:F129" ca="1" si="9">IF(ISERROR(D95),NA(),(D95-D94)/2+D94)</f>
@@ -26122,7 +26120,7 @@
       </c>
       <c r="K95" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L95" s="125"/>
       <c r="M95" s="85" t="b">
@@ -26299,11 +26297,11 @@
       </c>
       <c r="C96" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A96)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D96" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A96)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F96" s="103" t="e">
         <f t="shared" ca="1" si="9"/>
@@ -26323,7 +26321,7 @@
       </c>
       <c r="K96" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L96" s="125"/>
       <c r="M96" s="85" t="b">
@@ -26500,11 +26498,11 @@
       </c>
       <c r="C97" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A97)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D97" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A97)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F97" s="103" t="e">
         <f t="shared" ca="1" si="9"/>
@@ -26524,7 +26522,7 @@
       </c>
       <c r="K97" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L97" s="125"/>
       <c r="M97" s="85" t="b">
@@ -26701,11 +26699,11 @@
       </c>
       <c r="C98" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A98)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D98" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A98)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F98" s="103" t="e">
         <f t="shared" ca="1" si="9"/>
@@ -26725,7 +26723,7 @@
       </c>
       <c r="K98" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L98" s="125"/>
       <c r="M98" s="85" t="b">
@@ -26902,11 +26900,11 @@
       </c>
       <c r="C99" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A99)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D99" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A99)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F99" s="103" t="e">
         <f t="shared" ca="1" si="9"/>
@@ -26926,7 +26924,7 @@
       </c>
       <c r="K99" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L99" s="125"/>
       <c r="M99" s="85" t="b">
@@ -27103,11 +27101,11 @@
       </c>
       <c r="C100" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A100)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D100" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A100)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F100" s="103" t="e">
         <f t="shared" ca="1" si="9"/>
@@ -27127,7 +27125,7 @@
       </c>
       <c r="K100" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L100" s="125"/>
       <c r="M100" s="85" t="b">
@@ -27304,11 +27302,11 @@
       </c>
       <c r="C101" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A101)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D101" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A101)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F101" s="103" t="e">
         <f t="shared" ca="1" si="9"/>
@@ -27328,7 +27326,7 @@
       </c>
       <c r="K101" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L101" s="125"/>
       <c r="M101" s="85" t="b">
@@ -27505,11 +27503,11 @@
       </c>
       <c r="C102" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A102)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D102" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A102)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F102" s="103" t="e">
         <f t="shared" ca="1" si="9"/>
@@ -27529,7 +27527,7 @@
       </c>
       <c r="K102" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L102" s="125"/>
       <c r="M102" s="85" t="b">
@@ -27706,11 +27704,11 @@
       </c>
       <c r="C103" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A103)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D103" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A103)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F103" s="103" t="e">
         <f t="shared" ca="1" si="9"/>
@@ -27730,7 +27728,7 @@
       </c>
       <c r="K103" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L103" s="125"/>
       <c r="M103" s="85" t="b">
@@ -27907,11 +27905,11 @@
       </c>
       <c r="C104" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A104)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D104" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A104)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F104" s="103" t="e">
         <f t="shared" ca="1" si="9"/>
@@ -27931,7 +27929,7 @@
       </c>
       <c r="K104" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L104" s="125"/>
       <c r="M104" s="85" t="b">
@@ -28108,11 +28106,11 @@
       </c>
       <c r="C105" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A105)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D105" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A105)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F105" s="103" t="e">
         <f t="shared" ca="1" si="9"/>
@@ -28132,7 +28130,7 @@
       </c>
       <c r="K105" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L105" s="125"/>
       <c r="M105" s="85" t="b">
@@ -28309,11 +28307,11 @@
       </c>
       <c r="C106" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A106)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D106" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A106)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F106" s="103" t="e">
         <f t="shared" ca="1" si="9"/>
@@ -28333,7 +28331,7 @@
       </c>
       <c r="K106" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L106" s="125"/>
       <c r="M106" s="85" t="b">
@@ -28510,11 +28508,11 @@
       </c>
       <c r="C107" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A107)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D107" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A107)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F107" s="103" t="e">
         <f t="shared" ca="1" si="9"/>
@@ -28534,7 +28532,7 @@
       </c>
       <c r="K107" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L107" s="125"/>
       <c r="M107" s="85" t="b">
@@ -28711,11 +28709,11 @@
       </c>
       <c r="C108" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A108)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D108" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A108)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F108" s="103" t="e">
         <f t="shared" ca="1" si="9"/>
@@ -28735,7 +28733,7 @@
       </c>
       <c r="K108" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L108" s="125"/>
       <c r="M108" s="85" t="b">
@@ -28912,11 +28910,11 @@
       </c>
       <c r="C109" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A109)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D109" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A109)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F109" s="103" t="e">
         <f t="shared" ca="1" si="9"/>
@@ -28936,7 +28934,7 @@
       </c>
       <c r="K109" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L109" s="125"/>
       <c r="M109" s="85" t="b">
@@ -29113,11 +29111,11 @@
       </c>
       <c r="C110" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A110)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D110" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A110)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F110" s="103" t="e">
         <f t="shared" ca="1" si="9"/>
@@ -29137,7 +29135,7 @@
       </c>
       <c r="K110" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L110" s="125"/>
       <c r="M110" s="85" t="b">
@@ -29314,11 +29312,11 @@
       </c>
       <c r="C111" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A111)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D111" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A111)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F111" s="103" t="e">
         <f t="shared" ca="1" si="9"/>
@@ -29338,7 +29336,7 @@
       </c>
       <c r="K111" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L111" s="125"/>
       <c r="M111" s="85" t="b">
@@ -29515,11 +29513,11 @@
       </c>
       <c r="C112" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A112)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D112" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A112)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F112" s="103" t="e">
         <f t="shared" ca="1" si="9"/>
@@ -29539,7 +29537,7 @@
       </c>
       <c r="K112" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L112" s="125"/>
       <c r="M112" s="85" t="b">
@@ -29716,11 +29714,11 @@
       </c>
       <c r="C113" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A113)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D113" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A113)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F113" s="103" t="e">
         <f t="shared" ca="1" si="9"/>
@@ -29740,7 +29738,7 @@
       </c>
       <c r="K113" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L113" s="125"/>
       <c r="M113" s="85" t="b">
@@ -29917,11 +29915,11 @@
       </c>
       <c r="C114" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A114)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D114" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A114)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F114" s="103" t="e">
         <f t="shared" ca="1" si="9"/>
@@ -29941,7 +29939,7 @@
       </c>
       <c r="K114" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L114" s="125"/>
       <c r="M114" s="85" t="b">
@@ -30118,11 +30116,11 @@
       </c>
       <c r="C115" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A115)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D115" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A115)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F115" s="103" t="e">
         <f t="shared" ca="1" si="9"/>
@@ -30142,7 +30140,7 @@
       </c>
       <c r="K115" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L115" s="125"/>
       <c r="M115" s="85" t="b">
@@ -30319,11 +30317,11 @@
       </c>
       <c r="C116" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A116)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D116" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A116)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F116" s="103" t="e">
         <f t="shared" ca="1" si="9"/>
@@ -30343,7 +30341,7 @@
       </c>
       <c r="K116" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L116" s="125"/>
       <c r="M116" s="85" t="b">
@@ -30520,11 +30518,11 @@
       </c>
       <c r="C117" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A117)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D117" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A117)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F117" s="103" t="e">
         <f t="shared" ca="1" si="9"/>
@@ -30544,7 +30542,7 @@
       </c>
       <c r="K117" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L117" s="125"/>
       <c r="M117" s="85" t="b">
@@ -30721,11 +30719,11 @@
       </c>
       <c r="C118" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A118)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D118" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A118)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F118" s="103" t="e">
         <f t="shared" ca="1" si="9"/>
@@ -30745,7 +30743,7 @@
       </c>
       <c r="K118" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L118" s="125"/>
       <c r="M118" s="85" t="b">
@@ -30922,11 +30920,11 @@
       </c>
       <c r="C119" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A119)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D119" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A119)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F119" s="103" t="e">
         <f t="shared" ca="1" si="9"/>
@@ -30946,7 +30944,7 @@
       </c>
       <c r="K119" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L119" s="125"/>
       <c r="M119" s="85" t="b">
@@ -31123,11 +31121,11 @@
       </c>
       <c r="C120" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A120)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D120" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A120)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F120" s="103" t="e">
         <f t="shared" ca="1" si="9"/>
@@ -31147,7 +31145,7 @@
       </c>
       <c r="K120" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L120" s="125"/>
       <c r="M120" s="85" t="b">
@@ -31324,11 +31322,11 @@
       </c>
       <c r="C121" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A121)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D121" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A121)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F121" s="103" t="e">
         <f t="shared" ca="1" si="9"/>
@@ -31348,7 +31346,7 @@
       </c>
       <c r="K121" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L121" s="125"/>
       <c r="M121" s="85" t="b">
@@ -31525,11 +31523,11 @@
       </c>
       <c r="C122" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A122)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D122" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A122)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F122" s="103" t="e">
         <f t="shared" ca="1" si="9"/>
@@ -31549,7 +31547,7 @@
       </c>
       <c r="K122" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L122" s="125"/>
       <c r="M122" s="85" t="b">
@@ -31726,11 +31724,11 @@
       </c>
       <c r="C123" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A123)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D123" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A123)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F123" s="103" t="e">
         <f t="shared" ca="1" si="9"/>
@@ -31750,7 +31748,7 @@
       </c>
       <c r="K123" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L123" s="125"/>
       <c r="M123" s="85" t="b">
@@ -31927,11 +31925,11 @@
       </c>
       <c r="C124" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A124)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D124" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A124)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F124" s="103" t="e">
         <f t="shared" ca="1" si="9"/>
@@ -31951,7 +31949,7 @@
       </c>
       <c r="K124" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L124" s="125"/>
       <c r="M124" s="85" t="b">
@@ -32128,11 +32126,11 @@
       </c>
       <c r="C125" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A125)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D125" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A125)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F125" s="103" t="e">
         <f t="shared" ca="1" si="9"/>
@@ -32152,7 +32150,7 @@
       </c>
       <c r="K125" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L125" s="125"/>
       <c r="M125" s="85" t="b">
@@ -32329,11 +32327,11 @@
       </c>
       <c r="C126" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A126)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D126" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A126)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F126" s="103" t="e">
         <f t="shared" ca="1" si="9"/>
@@ -32353,7 +32351,7 @@
       </c>
       <c r="K126" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L126" s="125"/>
       <c r="M126" s="85" t="b">
@@ -32530,11 +32528,11 @@
       </c>
       <c r="C127" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A127)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D127" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A127)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F127" s="103" t="e">
         <f t="shared" ca="1" si="9"/>
@@ -32554,7 +32552,7 @@
       </c>
       <c r="K127" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L127" s="125"/>
       <c r="M127" s="85" t="b">
@@ -32731,11 +32729,11 @@
       </c>
       <c r="C128" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A128)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D128" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A128)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F128" s="103" t="e">
         <f t="shared" ca="1" si="9"/>
@@ -32755,7 +32753,7 @@
       </c>
       <c r="K128" s="113" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L128" s="125"/>
       <c r="M128" s="85" t="b">
@@ -32932,11 +32930,11 @@
       </c>
       <c r="C129" s="18" t="e">
         <f ca="1">_xll.qlRateHelperEarliestDate($A129)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="D129" s="19" t="e">
         <f ca="1">_xll.qlRateHelperLatestDate($A129)</f>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="F129" s="105" t="e">
         <f t="shared" ca="1" si="9"/>
@@ -32956,7 +32954,7 @@
       </c>
       <c r="K129" s="116" t="e">
         <f t="shared" ca="1" si="8"/>
-        <v>#NAME?</v>
+        <v>#NUM!</v>
       </c>
       <c r="L129" s="125"/>
       <c r="M129" s="90" t="b">
@@ -33142,7 +33140,9 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:R515"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -33182,7 +33182,7 @@
       <c r="L1" s="22"/>
       <c r="M1" s="23">
         <f ca="1">_xll.ohTrigger(M3:M4)</f>
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="N1" s="144"/>
     </row>
@@ -33256,7 +33256,7 @@
       </c>
       <c r="K3" s="40" t="str">
         <f>_xll.qlSimpleQuote(Trigger,J3,,TRUE)</f>
-        <v>EURJump1_SYNTHON_Quote#0004</v>
+        <v>EURJump1_SYNTHON_Quote#0002</v>
       </c>
       <c r="L3" s="40" t="e">
         <f t="array" aca="1" ref="L3:L15" ca="1">QuoteLive</f>
@@ -33308,7 +33308,7 @@
       </c>
       <c r="K4" s="141" t="str">
         <f>_xll.qlSimpleQuote(Trigger,J4,,TRUE)</f>
-        <v>EURJump2_SYNTHON_Quote#0004</v>
+        <v>EURJump2_SYNTHON_Quote#0002</v>
       </c>
       <c r="L4" s="141" t="e">
         <f ca="1"/>
@@ -33360,7 +33360,7 @@
       </c>
       <c r="K5" s="141" t="str">
         <f>_xll.qlSimpleQuote(Trigger,J5,,TRUE)</f>
-        <v>EURJump3_SYNTHON_Quote#0004</v>
+        <v>EURJump3_SYNTHON_Quote#0003</v>
       </c>
       <c r="L5" s="141" t="e">
         <f ca="1"/>
@@ -33412,7 +33412,7 @@
       </c>
       <c r="K6" s="141" t="str">
         <f>_xll.qlSimpleQuote(Trigger,J6,,TRUE)</f>
-        <v>EURJump4_SYNTHON_Quote#0004</v>
+        <v>EURJump4_SYNTHON_Quote#0002</v>
       </c>
       <c r="L6" s="141" t="e">
         <f ca="1"/>
@@ -33464,7 +33464,7 @@
       </c>
       <c r="K7" s="141" t="str">
         <f>_xll.qlSimpleQuote(Trigger,J7,,TRUE)</f>
-        <v>EURJump5_SYNTHON_Quote#0004</v>
+        <v>EURJump5_SYNTHON_Quote#0002</v>
       </c>
       <c r="L7" s="141" t="e">
         <f ca="1"/>
@@ -33516,7 +33516,7 @@
       </c>
       <c r="K8" s="141" t="str">
         <f>_xll.qlSimpleQuote(Trigger,J8,,TRUE)</f>
-        <v>EURJump6_SYNTHON_Quote#0004</v>
+        <v>EURJump6_SYNTHON_Quote#0002</v>
       </c>
       <c r="L8" s="141" t="e">
         <f ca="1"/>
@@ -33568,7 +33568,7 @@
       </c>
       <c r="K9" s="141" t="str">
         <f>_xll.qlSimpleQuote(Trigger,J9,,TRUE)</f>
-        <v>EURJump7_SYNTHON_Quote#0004</v>
+        <v>EURJump7_SYNTHON_Quote#0002</v>
       </c>
       <c r="L9" s="141" t="e">
         <f ca="1"/>
@@ -33620,7 +33620,7 @@
       </c>
       <c r="K10" s="141" t="str">
         <f>_xll.qlSimpleQuote(Trigger,J10,,TRUE)</f>
-        <v>EURJump8_SYNTHON_Quote#0004</v>
+        <v>EURJump8_SYNTHON_Quote#0002</v>
       </c>
       <c r="L10" s="141" t="e">
         <f ca="1"/>
@@ -33672,7 +33672,7 @@
       </c>
       <c r="K11" s="141" t="str">
         <f>_xll.qlSimpleQuote(Trigger,J11,,TRUE)</f>
-        <v>EURJump9_SYNTHON_Quote#0004</v>
+        <v>EURJump9_SYNTHON_Quote#0002</v>
       </c>
       <c r="L11" s="141" t="e">
         <f ca="1"/>
@@ -33724,7 +33724,7 @@
       </c>
       <c r="K12" s="141" t="str">
         <f>_xll.qlSimpleQuote(Trigger,J12,,TRUE)</f>
-        <v>EURJump10_SYNTHON_Quote#0004</v>
+        <v>EURJump10_SYNTHON_Quote#0002</v>
       </c>
       <c r="L12" s="141" t="e">
         <f ca="1"/>
@@ -33776,7 +33776,7 @@
       </c>
       <c r="K13" s="141" t="str">
         <f>_xll.qlSimpleQuote(Trigger,J13,,TRUE)</f>
-        <v>EURJump11_SYNTHON_Quote#0004</v>
+        <v>EURJump11_SYNTHON_Quote#0002</v>
       </c>
       <c r="L13" s="141" t="e">
         <f ca="1"/>
@@ -33828,7 +33828,7 @@
       </c>
       <c r="K14" s="141" t="str">
         <f>_xll.qlSimpleQuote(Trigger,J14,,TRUE)</f>
-        <v>EURJump12_SYNTHON_Quote#0004</v>
+        <v>EURJump12_SYNTHON_Quote#0002</v>
       </c>
       <c r="L14" s="141" t="e">
         <f ca="1"/>
@@ -33880,7 +33880,7 @@
       </c>
       <c r="K15" s="142" t="str">
         <f>_xll.qlSimpleQuote(Trigger,J15,,TRUE)</f>
-        <v>EURJump13_SYNTHON_Quote#0004</v>
+        <v>EURJump13_SYNTHON_Quote#0002</v>
       </c>
       <c r="L15" s="142" t="e">
         <f ca="1"/>

</xml_diff>

<commit_message>
replace anonymous objects with named ones (temporary workaround)
</commit_message>
<xml_diff>
--- a/Data2/XLS/EUR/EUR_JumpsQuotesFeedON.xlsx
+++ b/Data2/XLS/EUR/EUR_JumpsQuotesFeedON.xlsx
@@ -1677,11 +1677,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="400197888"/>
-        <c:axId val="400199680"/>
+        <c:axId val="389277184"/>
+        <c:axId val="389278720"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="400197888"/>
+        <c:axId val="389277184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1701,12 +1701,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="400199680"/>
+        <c:crossAx val="389278720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="400199680"/>
+        <c:axId val="389278720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1717,7 +1717,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="400197888"/>
+        <c:crossAx val="389277184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4874,11 +4874,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="400668928"/>
-        <c:axId val="400674816"/>
+        <c:axId val="390977024"/>
+        <c:axId val="390978560"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="400668928"/>
+        <c:axId val="390977024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4898,14 +4898,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="400674816"/>
+        <c:crossAx val="390978560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="400674816"/>
+        <c:axId val="390978560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4916,7 +4916,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="400668928"/>
+        <c:crossAx val="390977024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5048,7 +5048,7 @@
       <sheetData sheetId="0">
         <row r="6">
           <cell r="D6">
-            <v>3</v>
+            <v>1</v>
           </cell>
         </row>
       </sheetData>
@@ -5056,7 +5056,7 @@
       <sheetData sheetId="2">
         <row r="6">
           <cell r="D6" t="str">
-            <v>EUR6M#0002</v>
+            <v>EUR6M#0000</v>
           </cell>
         </row>
       </sheetData>
@@ -5091,7 +5091,7 @@
       <sheetData sheetId="7">
         <row r="6">
           <cell r="D6" t="str">
-            <v>EURTND_Quote#0002</v>
+            <v>EURTND_Quote#0000</v>
           </cell>
         </row>
       </sheetData>
@@ -5655,7 +5655,7 @@
         <v>65</v>
       </c>
       <c r="I7" s="61">
-        <v>42246.735532407409</v>
+        <v>42247.465601851851</v>
       </c>
       <c r="J7" s="58"/>
     </row>
@@ -5670,7 +5670,7 @@
       </c>
       <c r="I8" s="60">
         <f>[1]!TriggerCounter</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J8" s="58"/>
     </row>
@@ -5680,8 +5680,8 @@
         <v>14</v>
       </c>
       <c r="D9" s="54" t="str">
-        <f>_xll.qlPiecewiseYieldCurve(,,,,NDays,Calendar,_xll.ohPack(Calculation!A5:A129),DayCounter,,,Accuracy,TraitsID,InterpolatorID)</f>
-        <v>obj_00504#0002</v>
+        <f>_xll.qlPiecewiseYieldCurve(,"yc1",,,NDays,Calendar,_xll.ohPack(Calculation!A5:A129),DayCounter,,,Accuracy,TraitsID,InterpolatorID)</f>
+        <v>yc1#0001</v>
       </c>
       <c r="E9" s="4"/>
       <c r="G9" s="1"/>
@@ -5690,7 +5690,7 @@
       </c>
       <c r="I9" s="29">
         <f>_xll.ohTrigger(Contribution!M1)</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J9" s="4"/>
     </row>
@@ -5763,8 +5763,8 @@
         <v>14</v>
       </c>
       <c r="I14" s="54" t="str">
-        <f>_xll.qlPiecewiseYieldCurve(,,,,NDays,Calendar,_xll.ohPack(Calculation!A5:A129),DayCounter,JumpQuotes,JumpDates,Accuracy,TraitsID,InterpolatorID)</f>
-        <v>obj_00506#0002</v>
+        <f>_xll.qlPiecewiseYieldCurve(,"yc2",,,NDays,Calendar,_xll.ohPack(Calculation!A5:A129),DayCounter,JumpQuotes,JumpDates,Accuracy,TraitsID,InterpolatorID)</f>
+        <v>yc2#0002</v>
       </c>
       <c r="J14" s="4"/>
     </row>
@@ -5801,8 +5801,8 @@
         <v>97</v>
       </c>
       <c r="I16" s="174" t="str">
-        <f>_xll.qlEonia(,,,,$I$14)</f>
-        <v>obj_00507#0002</v>
+        <f>_xll.qlEonia(,"id1",,,$I$14)</f>
+        <v>id1#0003</v>
       </c>
       <c r="J16" s="4"/>
     </row>
@@ -6015,7 +6015,7 @@
       </c>
       <c r="F2" s="77" t="str">
         <f>_xll.qlFraRateHelper(EvaluationDate,"W"&amp;Currency&amp;B2&amp;C2&amp;D2,,,E2,"2d",OvernightIndex)</f>
-        <v>WEURSND#0002</v>
+        <v>WEURSND#0000</v>
       </c>
       <c r="G2" s="78" t="b">
         <v>0</v>
@@ -6056,7 +6056,7 @@
       </c>
       <c r="F3" s="81" t="str">
         <f>_xll.qlDatedOISRateHelper(,"W"&amp;Currency&amp;B3&amp;C3&amp;D3,,,A3,A4,E3,OvernightIndex)</f>
-        <v>WEURECBOISJUN15#0002</v>
+        <v>WEURECBOISJUN15#0000</v>
       </c>
       <c r="G3" s="82" t="b">
         <f>IF(ISERROR(F3),FALSE,TRUE)</f>
@@ -6099,7 +6099,7 @@
       </c>
       <c r="F4" s="85" t="str">
         <f>_xll.qlDatedOISRateHelper(,"W"&amp;Currency&amp;B4&amp;C4&amp;D4,,,A4,A5,E4,OvernightIndex)</f>
-        <v>WEURECBOISJUL15#0002</v>
+        <v>WEURECBOISJUL15#0000</v>
       </c>
       <c r="G4" s="82" t="b">
         <f t="shared" ref="G4:G12" si="1">IF(ISERROR(F4),FALSE,TRUE)</f>
@@ -6142,7 +6142,7 @@
       </c>
       <c r="F5" s="85" t="str">
         <f>_xll.qlDatedOISRateHelper(,"W"&amp;Currency&amp;B5&amp;C5&amp;D5,,,A5,A6,E5,OvernightIndex)</f>
-        <v>WEURECBOISSEP15#0002</v>
+        <v>WEURECBOISSEP15#0000</v>
       </c>
       <c r="G5" s="82" t="b">
         <f t="shared" si="1"/>
@@ -6184,7 +6184,7 @@
       </c>
       <c r="F6" s="85" t="str">
         <f>_xll.qlDatedOISRateHelper(,"W"&amp;Currency&amp;B6&amp;C6&amp;D6,,,A6,A7,E6,OvernightIndex)</f>
-        <v>WEURECBOISOCT15#0002</v>
+        <v>WEURECBOISOCT15#0000</v>
       </c>
       <c r="G6" s="82" t="b">
         <f t="shared" si="1"/>
@@ -6226,7 +6226,7 @@
       </c>
       <c r="F7" s="85" t="str">
         <f>_xll.qlDatedOISRateHelper(,"W"&amp;Currency&amp;B7&amp;C7&amp;D7,,,A7,A8,E7,OvernightIndex)</f>
-        <v>WEURECBOISDEC15#0002</v>
+        <v>WEURECBOISDEC15#0000</v>
       </c>
       <c r="G7" s="82" t="b">
         <f t="shared" si="1"/>
@@ -6268,7 +6268,7 @@
       </c>
       <c r="F8" s="85" t="str">
         <f>_xll.qlDatedOISRateHelper(,"W"&amp;Currency&amp;B8&amp;C8&amp;D8,,,A8,A9,E8,OvernightIndex)</f>
-        <v>WEURECBOISJAN16#0002</v>
+        <v>WEURECBOISJAN16#0000</v>
       </c>
       <c r="G8" s="82" t="b">
         <f t="shared" si="1"/>
@@ -6310,7 +6310,7 @@
       </c>
       <c r="F9" s="85" t="str">
         <f>_xll.qlDatedOISRateHelper(,"W"&amp;Currency&amp;B9&amp;C9&amp;D9,,,A9,A10,E9,OvernightIndex)</f>
-        <v>WEURECBOISMAR16#0002</v>
+        <v>WEURECBOISMAR16#0000</v>
       </c>
       <c r="G9" s="82" t="b">
         <f t="shared" si="1"/>
@@ -6352,7 +6352,7 @@
       </c>
       <c r="F10" s="85" t="str">
         <f>_xll.qlDatedOISRateHelper(,"W"&amp;Currency&amp;B10&amp;C10&amp;D10,,,A10,A11,E10,OvernightIndex)</f>
-        <v>WEURECBOISAPR16#0002</v>
+        <v>WEURECBOISAPR16#0000</v>
       </c>
       <c r="G10" s="82" t="b">
         <f t="shared" si="1"/>
@@ -6659,7 +6659,7 @@
       </c>
       <c r="F18" s="81" t="str">
         <f>_xll.qlOISRateHelper(EvaluationDate,"W"&amp;Currency&amp;B18&amp;C18&amp;D18,,,2,"1w",E18,OvernightIndex)</f>
-        <v>WEUREONSW#0002</v>
+        <v>WEUREONSW#0000</v>
       </c>
       <c r="G18" s="83" t="b">
         <v>1</v>
@@ -6694,7 +6694,7 @@
       </c>
       <c r="F19" s="85" t="str">
         <f>_xll.qlOISRateHelper(EvaluationDate,"W"&amp;Currency&amp;B19&amp;C19&amp;D19,,,2,D19,E19,OvernightIndex)</f>
-        <v>WEUREON2W#0002</v>
+        <v>WEUREON2W#0000</v>
       </c>
       <c r="G19" s="82" t="b">
         <v>1</v>
@@ -6729,7 +6729,7 @@
       </c>
       <c r="F20" s="85" t="str">
         <f>_xll.qlOISRateHelper(EvaluationDate,"W"&amp;Currency&amp;B20&amp;C20&amp;D20,,,2,D20,E20,OvernightIndex)</f>
-        <v>WEUREON3W#0002</v>
+        <v>WEUREON3W#0000</v>
       </c>
       <c r="G20" s="82" t="b">
         <v>1</v>
@@ -6764,7 +6764,7 @@
       </c>
       <c r="F21" s="85" t="str">
         <f>_xll.qlOISRateHelper(EvaluationDate,"W"&amp;Currency&amp;B21&amp;C21&amp;D21,,,2,D21,E21,OvernightIndex)</f>
-        <v>WEUREON1M#0002</v>
+        <v>WEUREON1M#0000</v>
       </c>
       <c r="G21" s="82" t="b">
         <v>1</v>
@@ -6799,7 +6799,7 @@
       </c>
       <c r="F22" s="85" t="str">
         <f>_xll.qlOISRateHelper(EvaluationDate,"W"&amp;Currency&amp;B22&amp;C22&amp;D22,,,2,D22,E22,OvernightIndex)</f>
-        <v>WEUREON2M#0002</v>
+        <v>WEUREON2M#0000</v>
       </c>
       <c r="G22" s="82" t="b">
         <v>1</v>
@@ -6834,7 +6834,7 @@
       </c>
       <c r="F23" s="85" t="str">
         <f>_xll.qlOISRateHelper(EvaluationDate,"W"&amp;Currency&amp;B23&amp;C23&amp;D23,,,2,D23,E23,OvernightIndex)</f>
-        <v>WEUREON3M#0002</v>
+        <v>WEUREON3M#0000</v>
       </c>
       <c r="G23" s="82" t="b">
         <v>1</v>
@@ -6869,7 +6869,7 @@
       </c>
       <c r="F24" s="85" t="str">
         <f>_xll.qlOISRateHelper(EvaluationDate,"W"&amp;Currency&amp;B24&amp;C24&amp;D24,,,2,D24,E24,OvernightIndex)</f>
-        <v>WEUREON4M#0002</v>
+        <v>WEUREON4M#0000</v>
       </c>
       <c r="G24" s="82" t="b">
         <v>1</v>
@@ -6904,7 +6904,7 @@
       </c>
       <c r="F25" s="85" t="str">
         <f>_xll.qlOISRateHelper(EvaluationDate,"W"&amp;Currency&amp;B25&amp;C25&amp;D25,,,2,D25,E25,OvernightIndex)</f>
-        <v>WEUREON5M#0002</v>
+        <v>WEUREON5M#0000</v>
       </c>
       <c r="G25" s="82" t="b">
         <v>1</v>
@@ -6939,7 +6939,7 @@
       </c>
       <c r="F26" s="85" t="str">
         <f>_xll.qlOISRateHelper(EvaluationDate,"W"&amp;Currency&amp;B26&amp;C26&amp;D26,,,2,D26,E26,OvernightIndex)</f>
-        <v>WEUREON6M#0002</v>
+        <v>WEUREON6M#0000</v>
       </c>
       <c r="G26" s="82" t="b">
         <v>1</v>
@@ -6974,7 +6974,7 @@
       </c>
       <c r="F27" s="85" t="str">
         <f>_xll.qlOISRateHelper(EvaluationDate,"W"&amp;Currency&amp;B27&amp;C27&amp;D27,,,2,D27,E27,OvernightIndex)</f>
-        <v>WEUREON7M#0002</v>
+        <v>WEUREON7M#0000</v>
       </c>
       <c r="G27" s="82" t="b">
         <v>1</v>
@@ -7009,7 +7009,7 @@
       </c>
       <c r="F28" s="85" t="str">
         <f>_xll.qlOISRateHelper(EvaluationDate,"W"&amp;Currency&amp;B28&amp;C28&amp;D28,,,2,D28,E28,OvernightIndex)</f>
-        <v>WEUREON8M#0002</v>
+        <v>WEUREON8M#0000</v>
       </c>
       <c r="G28" s="82" t="b">
         <v>1</v>
@@ -7044,7 +7044,7 @@
       </c>
       <c r="F29" s="85" t="str">
         <f>_xll.qlOISRateHelper(EvaluationDate,"W"&amp;Currency&amp;B29&amp;C29&amp;D29,,,2,D29,E29,OvernightIndex)</f>
-        <v>WEUREON9M#0002</v>
+        <v>WEUREON9M#0000</v>
       </c>
       <c r="G29" s="82" t="b">
         <v>1</v>
@@ -7079,7 +7079,7 @@
       </c>
       <c r="F30" s="85" t="str">
         <f>_xll.qlOISRateHelper(EvaluationDate,"W"&amp;Currency&amp;B30&amp;C30&amp;D30,,,2,D30,E30,OvernightIndex)</f>
-        <v>WEUREON10M#0002</v>
+        <v>WEUREON10M#0000</v>
       </c>
       <c r="G30" s="82" t="b">
         <v>1</v>
@@ -7114,7 +7114,7 @@
       </c>
       <c r="F31" s="85" t="str">
         <f>_xll.qlOISRateHelper(EvaluationDate,"W"&amp;Currency&amp;B31&amp;C31&amp;D31,,,2,D31,E31,OvernightIndex)</f>
-        <v>WEUREON11M#0002</v>
+        <v>WEUREON11M#0000</v>
       </c>
       <c r="G31" s="82" t="b">
         <v>1</v>
@@ -7149,7 +7149,7 @@
       </c>
       <c r="F32" s="85" t="str">
         <f>_xll.qlOISRateHelper(EvaluationDate,"W"&amp;Currency&amp;B32&amp;C32&amp;D32,,,2,D32,E32,OvernightIndex)</f>
-        <v>WEUREON1Y#0002</v>
+        <v>WEUREON1Y#0000</v>
       </c>
       <c r="G32" s="82" t="b">
         <v>1</v>
@@ -7184,7 +7184,7 @@
       </c>
       <c r="F33" s="85" t="str">
         <f>_xll.qlOISRateHelper(EvaluationDate,"W"&amp;Currency&amp;B33&amp;C33&amp;D33,,,2,D33,E33,OvernightIndex)</f>
-        <v>WEUREON15M#0002</v>
+        <v>WEUREON15M#0000</v>
       </c>
       <c r="G33" s="82" t="b">
         <v>1</v>
@@ -7219,7 +7219,7 @@
       </c>
       <c r="F34" s="85" t="str">
         <f>_xll.qlOISRateHelper(EvaluationDate,"W"&amp;Currency&amp;B34&amp;C34&amp;D34,,,2,D34,E34,OvernightIndex)</f>
-        <v>WEUREON18M#0002</v>
+        <v>WEUREON18M#0000</v>
       </c>
       <c r="G34" s="82" t="b">
         <v>1</v>
@@ -7254,7 +7254,7 @@
       </c>
       <c r="F35" s="85" t="str">
         <f>_xll.qlOISRateHelper(EvaluationDate,"W"&amp;Currency&amp;B35&amp;C35&amp;D35,,,2,D35,E35,OvernightIndex)</f>
-        <v>WEUREON21M#0002</v>
+        <v>WEUREON21M#0000</v>
       </c>
       <c r="G35" s="82" t="b">
         <v>1</v>
@@ -7289,7 +7289,7 @@
       </c>
       <c r="F36" s="90" t="str">
         <f>_xll.qlOISRateHelper(EvaluationDate,"W"&amp;Currency&amp;B36&amp;C36&amp;D36,,,2,D36,E36,OvernightIndex)</f>
-        <v>WEUREON2Y#0002</v>
+        <v>WEUREON2Y#0000</v>
       </c>
       <c r="G36" s="91" t="b">
         <v>1</v>
@@ -7322,35 +7322,35 @@
     <row r="38" spans="2:11" x14ac:dyDescent="0.2">
       <c r="D38" s="93">
         <f>_xll.ohTrigger(RateHelpers)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E38" s="93">
         <f>_xll.ohTrigger(RateHelpers)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F38" s="93">
         <f>_xll.ohTrigger(RateHelpers)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G38" s="93">
         <f>_xll.ohTrigger(RateHelpers)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H38" s="93">
         <f>_xll.ohTrigger(RateHelpers)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I38" s="93">
         <f>_xll.ohTrigger(RateHelpers)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J38" s="93">
         <f>_xll.ohTrigger(RateHelpers)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K38" s="93">
         <f>_xll.ohTrigger(RateHelpers)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.2">
@@ -7730,8 +7730,8 @@
       </c>
       <c r="L3" s="125"/>
       <c r="M3" s="107" t="str">
-        <f>_xll.qlGenericInterp(,,,,FwdInterpolation,_xll.ohFilter($F5:$F129,M5:M129),_xll.ohFilter(J5:J129,M5:M129))</f>
-        <v>obj_00505#0002</v>
+        <f>_xll.qlGenericInterp(,"interp1",,,FwdInterpolation,_xll.ohFilter($F5:$F129,M5:M129),_xll.ohFilter(J5:J129,M5:M129))</f>
+        <v>interp1#0002</v>
       </c>
       <c r="N3" s="118" t="s">
         <v>67</v>
@@ -7741,8 +7741,8 @@
       </c>
       <c r="P3" s="126"/>
       <c r="Q3" s="107" t="str">
-        <f>_xll.qlGenericInterp(,,,,FwdInterpolation,_xll.ohFilter($F5:$F129,Q5:Q129),_xll.ohFilter(N5:N129,Q5:Q129))</f>
-        <v>obj_00508#0002</v>
+        <f>_xll.qlGenericInterp(,"interp2",,,FwdInterpolation,_xll.ohFilter($F5:$F129,Q5:Q129),_xll.ohFilter(N5:N129,Q5:Q129))</f>
+        <v>interp2#0003</v>
       </c>
       <c r="R3" s="118" t="s">
         <v>67</v>
@@ -7752,8 +7752,8 @@
       </c>
       <c r="T3" s="127"/>
       <c r="U3" s="107" t="str">
-        <f>_xll.qlGenericInterp(,,,,FwdInterpolation,_xll.ohFilter($F5:$F129,U5:U129),_xll.ohFilter(R5:R129,U5:U129))</f>
-        <v>obj_00509#0002</v>
+        <f>_xll.qlGenericInterp(,"interp3",,,FwdInterpolation,_xll.ohFilter($F5:$F129,U5:U129),_xll.ohFilter(R5:R129,U5:U129))</f>
+        <v>interp3#0004</v>
       </c>
       <c r="V3" s="118" t="s">
         <v>67</v>
@@ -7763,8 +7763,8 @@
       </c>
       <c r="X3" s="127"/>
       <c r="Y3" s="107" t="str">
-        <f>_xll.qlGenericInterp(,,,,FwdInterpolation,_xll.ohFilter($F5:$F129,Y5:Y129),_xll.ohFilter(V5:V129,Y5:Y129))</f>
-        <v>obj_0050a#0002</v>
+        <f>_xll.qlGenericInterp(,"interp4",,,FwdInterpolation,_xll.ohFilter($F5:$F129,Y5:Y129),_xll.ohFilter(V5:V129,Y5:Y129))</f>
+        <v>interp4#0005</v>
       </c>
       <c r="Z3" s="118" t="s">
         <v>67</v>
@@ -7774,8 +7774,8 @@
       </c>
       <c r="AB3" s="127"/>
       <c r="AC3" s="107" t="str">
-        <f>_xll.qlGenericInterp(,,,,FwdInterpolation,_xll.ohFilter($F5:$F129,AC5:AC129),_xll.ohFilter(Z5:Z129,AC5:AC129))</f>
-        <v>obj_0050b#0002</v>
+        <f>_xll.qlGenericInterp(,"interp5",,,FwdInterpolation,_xll.ohFilter($F5:$F129,AC5:AC129),_xll.ohFilter(Z5:Z129,AC5:AC129))</f>
+        <v>interp5#0006</v>
       </c>
       <c r="AD3" s="118" t="s">
         <v>67</v>
@@ -7785,8 +7785,8 @@
       </c>
       <c r="AF3" s="127"/>
       <c r="AG3" s="107" t="str">
-        <f>_xll.qlGenericInterp(,,,,FwdInterpolation,_xll.ohFilter($F5:$F129,AG5:AG129),_xll.ohFilter(AD5:AD129,AG5:AG129))</f>
-        <v>obj_0050c#0002</v>
+        <f>_xll.qlGenericInterp(,"interp6",,,FwdInterpolation,_xll.ohFilter($F5:$F129,AG5:AG129),_xll.ohFilter(AD5:AD129,AG5:AG129))</f>
+        <v>interp6#0007</v>
       </c>
       <c r="AH3" s="118" t="s">
         <v>67</v>
@@ -7796,8 +7796,8 @@
       </c>
       <c r="AJ3" s="127"/>
       <c r="AK3" s="107" t="str">
-        <f>_xll.qlGenericInterp(,,,,FwdInterpolation,_xll.ohFilter($F5:$F129,AK5:AK129),_xll.ohFilter(AH5:AH129,AK5:AK129))</f>
-        <v>obj_0050d#0002</v>
+        <f>_xll.qlGenericInterp(,"interp7",,,FwdInterpolation,_xll.ohFilter($F5:$F129,AK5:AK129),_xll.ohFilter(AH5:AH129,AK5:AK129))</f>
+        <v>interp7#0008</v>
       </c>
       <c r="AL3" s="118" t="s">
         <v>67</v>
@@ -7806,8 +7806,8 @@
         <v>69</v>
       </c>
       <c r="AO3" s="107" t="str">
-        <f>_xll.qlGenericInterp(,,,,FwdInterpolation,_xll.ohFilter($F5:$F129,AO5:AO129),_xll.ohFilter(AL5:AL129,AO5:AO129))</f>
-        <v>obj_0050e#0002</v>
+        <f>_xll.qlGenericInterp(,"interp8",,,FwdInterpolation,_xll.ohFilter($F5:$F129,AO5:AO129),_xll.ohFilter(AL5:AL129,AO5:AO129))</f>
+        <v>interp8#0009</v>
       </c>
       <c r="AP3" s="118" t="s">
         <v>67</v>
@@ -7816,8 +7816,8 @@
         <v>69</v>
       </c>
       <c r="AS3" s="107" t="str">
-        <f>_xll.qlGenericInterp(,,,,FwdInterpolation,_xll.ohFilter($F5:$F129,AS5:AS129),_xll.ohFilter(AP5:AP129,AS5:AS129))</f>
-        <v>obj_0050f#0002</v>
+        <f>_xll.qlGenericInterp(,"interp9",,,FwdInterpolation,_xll.ohFilter($F5:$F129,AS5:AS129),_xll.ohFilter(AP5:AP129,AS5:AS129))</f>
+        <v>interp9#0010</v>
       </c>
       <c r="AT3" s="118" t="s">
         <v>67</v>
@@ -7826,8 +7826,8 @@
         <v>69</v>
       </c>
       <c r="AW3" s="107" t="str">
-        <f>_xll.qlGenericInterp(,,,,FwdInterpolation,_xll.ohFilter($F5:$F129,AW5:AW129),_xll.ohFilter(AT5:AT129,AW5:AW129))</f>
-        <v>obj_00510#0002</v>
+        <f>_xll.qlGenericInterp(,"interp10",,,FwdInterpolation,_xll.ohFilter($F5:$F129,AW5:AW129),_xll.ohFilter(AT5:AT129,AW5:AW129))</f>
+        <v>interp10#0011</v>
       </c>
       <c r="AX3" s="118" t="s">
         <v>67</v>
@@ -7836,8 +7836,8 @@
         <v>69</v>
       </c>
       <c r="BA3" s="107" t="str">
-        <f>_xll.qlGenericInterp(,,,,FwdInterpolation,_xll.ohFilter($F5:$F129,BA5:BA129),_xll.ohFilter(AX5:AX129,BA5:BA129))</f>
-        <v>obj_00511#0002</v>
+        <f>_xll.qlGenericInterp(,"interp11",,,FwdInterpolation,_xll.ohFilter($F5:$F129,BA5:BA129),_xll.ohFilter(AX5:AX129,BA5:BA129))</f>
+        <v>interp11#0012</v>
       </c>
       <c r="BB3" s="118" t="s">
         <v>67</v>
@@ -7846,8 +7846,8 @@
         <v>69</v>
       </c>
       <c r="BE3" s="107" t="str">
-        <f>_xll.qlGenericInterp(,,,,FwdInterpolation,_xll.ohFilter($F5:$F129,BE5:BE129),_xll.ohFilter(BB5:BB129,BE5:BE129))</f>
-        <v>obj_00512#0002</v>
+        <f>_xll.qlGenericInterp(,"interp12",,,FwdInterpolation,_xll.ohFilter($F5:$F129,BE5:BE129),_xll.ohFilter(BB5:BB129,BE5:BE129))</f>
+        <v>interp12#0013</v>
       </c>
       <c r="BF3" s="118" t="s">
         <v>67</v>
@@ -7856,8 +7856,8 @@
         <v>69</v>
       </c>
       <c r="BI3" s="107" t="str">
-        <f>_xll.qlGenericInterp(,,,,FwdInterpolation,_xll.ohFilter($F5:$F129,BI5:BI129),_xll.ohFilter(BF5:BF129,BI5:BI129))</f>
-        <v>obj_00513#0002</v>
+        <f>_xll.qlGenericInterp(,"interp13",,,FwdInterpolation,_xll.ohFilter($F5:$F129,BI5:BI129),_xll.ohFilter(BF5:BF129,BI5:BI129))</f>
+        <v>interp13#0014</v>
       </c>
       <c r="BJ3" s="118" t="s">
         <v>67</v>
@@ -32936,7 +32936,7 @@
       <c r="L1" s="22"/>
       <c r="M1" s="23">
         <f>_xll.ohTrigger(M3:M4)</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="N1" s="144"/>
     </row>
@@ -33010,7 +33010,7 @@
       </c>
       <c r="K3" s="40" t="str">
         <f>_xll.qlSimpleQuote(Trigger,J3,,TRUE)</f>
-        <v>EURJump1_SYNTHON_Quote#0002</v>
+        <v>EURJump1_SYNTHON_Quote#0000</v>
       </c>
       <c r="L3" s="40">
         <f t="array" ref="L3:L15">QuoteStatic</f>
@@ -33062,7 +33062,7 @@
       </c>
       <c r="K4" s="141" t="str">
         <f>_xll.qlSimpleQuote(Trigger,J4,,TRUE)</f>
-        <v>EURJump2_SYNTHON_Quote#0002</v>
+        <v>EURJump2_SYNTHON_Quote#0000</v>
       </c>
       <c r="L4" s="141">
         <v>1</v>
@@ -33113,7 +33113,7 @@
       </c>
       <c r="K5" s="141" t="str">
         <f>_xll.qlSimpleQuote(Trigger,J5,,TRUE)</f>
-        <v>EURJump3_SYNTHON_Quote#0002</v>
+        <v>EURJump3_SYNTHON_Quote#0000</v>
       </c>
       <c r="L5" s="141">
         <v>0.99999685161729968</v>
@@ -33164,7 +33164,7 @@
       </c>
       <c r="K6" s="141" t="str">
         <f>_xll.qlSimpleQuote(Trigger,J6,,TRUE)</f>
-        <v>EURJump4_SYNTHON_Quote#0002</v>
+        <v>EURJump4_SYNTHON_Quote#0000</v>
       </c>
       <c r="L6" s="141">
         <v>0.99999237575302491</v>
@@ -33215,7 +33215,7 @@
       </c>
       <c r="K7" s="141" t="str">
         <f>_xll.qlSimpleQuote(Trigger,J7,,TRUE)</f>
-        <v>EURJump5_SYNTHON_Quote#0002</v>
+        <v>EURJump5_SYNTHON_Quote#0000</v>
       </c>
       <c r="L7" s="141">
         <v>0.99996824223590031</v>
@@ -33266,7 +33266,7 @@
       </c>
       <c r="K8" s="141" t="str">
         <f>_xll.qlSimpleQuote(Trigger,J8,,TRUE)</f>
-        <v>EURJump6_SYNTHON_Quote#0002</v>
+        <v>EURJump6_SYNTHON_Quote#0000</v>
       </c>
       <c r="L8" s="141">
         <v>0.99997651632635709</v>
@@ -33317,7 +33317,7 @@
       </c>
       <c r="K9" s="141" t="str">
         <f>_xll.qlSimpleQuote(Trigger,J9,,TRUE)</f>
-        <v>EURJump7_SYNTHON_Quote#0002</v>
+        <v>EURJump7_SYNTHON_Quote#0000</v>
       </c>
       <c r="L9" s="141">
         <v>0.99998988369315134</v>
@@ -33368,7 +33368,7 @@
       </c>
       <c r="K10" s="141" t="str">
         <f>_xll.qlSimpleQuote(Trigger,J10,,TRUE)</f>
-        <v>EURJump8_SYNTHON_Quote#0002</v>
+        <v>EURJump8_SYNTHON_Quote#0000</v>
       </c>
       <c r="L10" s="141">
         <v>0.99999226871935276</v>
@@ -33419,7 +33419,7 @@
       </c>
       <c r="K11" s="141" t="str">
         <f>_xll.qlSimpleQuote(Trigger,J11,,TRUE)</f>
-        <v>EURJump9_SYNTHON_Quote#0002</v>
+        <v>EURJump9_SYNTHON_Quote#0000</v>
       </c>
       <c r="L11" s="141">
         <v>0.99999360896660505</v>
@@ -33470,7 +33470,7 @@
       </c>
       <c r="K12" s="141" t="str">
         <f>_xll.qlSimpleQuote(Trigger,J12,,TRUE)</f>
-        <v>EURJump10_SYNTHON_Quote#0002</v>
+        <v>EURJump10_SYNTHON_Quote#0000</v>
       </c>
       <c r="L12" s="141">
         <v>0.99999659453552103</v>
@@ -33521,7 +33521,7 @@
       </c>
       <c r="K13" s="141" t="str">
         <f>_xll.qlSimpleQuote(Trigger,J13,,TRUE)</f>
-        <v>EURJump11_SYNTHON_Quote#0002</v>
+        <v>EURJump11_SYNTHON_Quote#0000</v>
       </c>
       <c r="L13" s="141">
         <v>0.99999880458778456</v>
@@ -33572,7 +33572,7 @@
       </c>
       <c r="K14" s="141" t="str">
         <f>_xll.qlSimpleQuote(Trigger,J14,,TRUE)</f>
-        <v>EURJump12_SYNTHON_Quote#0002</v>
+        <v>EURJump12_SYNTHON_Quote#0000</v>
       </c>
       <c r="L14" s="141">
         <v>1</v>
@@ -33623,7 +33623,7 @@
       </c>
       <c r="K15" s="142" t="str">
         <f>_xll.qlSimpleQuote(Trigger,J15,,TRUE)</f>
-        <v>EURJump13_SYNTHON_Quote#0002</v>
+        <v>EURJump13_SYNTHON_Quote#0000</v>
       </c>
       <c r="L15" s="142">
         <v>0.99996612432397214</v>

</xml_diff>